<commit_message>
changed Simplifiedwords_grouped_into_POS (.xlsx and .csv)
</commit_message>
<xml_diff>
--- a/Simplifiedwords_grouped_into_POS.xlsx
+++ b/Simplifiedwords_grouped_into_POS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5252" uniqueCount="4616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5249" uniqueCount="4616">
   <si>
     <t>a</t>
   </si>
@@ -12509,9 +12509,6 @@
     <t>not found</t>
   </si>
   <si>
-    <t>don't</t>
-  </si>
-  <si>
     <t>nowadays</t>
   </si>
   <si>
@@ -13412,9 +13409,6 @@
     <t>encouragement</t>
   </si>
   <si>
-    <t>hon.</t>
-  </si>
-  <si>
     <t>machinery</t>
   </si>
   <si>
@@ -13872,6 +13866,12 @@
   </si>
   <si>
     <t>delegation</t>
+  </si>
+  <si>
+    <t>its</t>
+  </si>
+  <si>
+    <t>us</t>
   </si>
 </sst>
 </file>
@@ -14201,7 +14201,7 @@
   <dimension ref="A1:P2459"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+      <selection activeCell="C4" sqref="A1:P2459"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14452,7 +14452,7 @@
         <v>3558</v>
       </c>
       <c r="P6" t="s">
-        <v>4165</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
@@ -14490,7 +14490,7 @@
         <v>2247</v>
       </c>
       <c r="P7" t="s">
-        <v>82</v>
+        <v>4165</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
@@ -14528,12 +14528,12 @@
         <v>3559</v>
       </c>
       <c r="P8" t="s">
-        <v>869</v>
+        <v>4166</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>7</v>
+        <v>4614</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
@@ -14566,12 +14566,12 @@
         <v>3560</v>
       </c>
       <c r="P9" t="s">
-        <v>874</v>
+        <v>4167</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
         <v>20</v>
@@ -14604,12 +14604,12 @@
         <v>3561</v>
       </c>
       <c r="P10" t="s">
-        <v>875</v>
+        <v>4168</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
         <v>21</v>
@@ -14642,10 +14642,13 @@
         <v>3562</v>
       </c>
       <c r="P11" t="s">
-        <v>4166</v>
+        <v>4169</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
       <c r="C12" t="s">
         <v>22</v>
       </c>
@@ -14677,7 +14680,7 @@
         <v>1541</v>
       </c>
       <c r="P12" t="s">
-        <v>4167</v>
+        <v>4170</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.35">
@@ -14712,7 +14715,7 @@
         <v>3563</v>
       </c>
       <c r="P13" t="s">
-        <v>4168</v>
+        <v>4171</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.35">
@@ -14735,7 +14738,7 @@
         <v>923</v>
       </c>
       <c r="J14" t="s">
-        <v>3285</v>
+        <v>4615</v>
       </c>
       <c r="K14" t="s">
         <v>284</v>
@@ -14744,7 +14747,7 @@
         <v>3564</v>
       </c>
       <c r="P14" t="s">
-        <v>4169</v>
+        <v>4172</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.35">
@@ -14767,7 +14770,7 @@
         <v>924</v>
       </c>
       <c r="J15" t="s">
-        <v>3286</v>
+        <v>3285</v>
       </c>
       <c r="K15" t="s">
         <v>31</v>
@@ -14776,7 +14779,7 @@
         <v>3565</v>
       </c>
       <c r="P15" t="s">
-        <v>4170</v>
+        <v>4173</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.35">
@@ -14799,7 +14802,7 @@
         <v>925</v>
       </c>
       <c r="J16" t="s">
-        <v>3287</v>
+        <v>3286</v>
       </c>
       <c r="K16" t="s">
         <v>983</v>
@@ -14808,7 +14811,7 @@
         <v>3566</v>
       </c>
       <c r="P16" t="s">
-        <v>4171</v>
+        <v>4174</v>
       </c>
     </row>
     <row r="17" spans="3:16" x14ac:dyDescent="0.35">
@@ -14831,7 +14834,7 @@
         <v>926</v>
       </c>
       <c r="J17" t="s">
-        <v>3288</v>
+        <v>3287</v>
       </c>
       <c r="K17" t="s">
         <v>81</v>
@@ -14840,7 +14843,7 @@
         <v>3567</v>
       </c>
       <c r="P17" t="s">
-        <v>4172</v>
+        <v>4175</v>
       </c>
     </row>
     <row r="18" spans="3:16" x14ac:dyDescent="0.35">
@@ -14863,7 +14866,7 @@
         <v>927</v>
       </c>
       <c r="J18" t="s">
-        <v>3289</v>
+        <v>3288</v>
       </c>
       <c r="K18" t="s">
         <v>121</v>
@@ -14872,7 +14875,7 @@
         <v>3568</v>
       </c>
       <c r="P18" t="s">
-        <v>4173</v>
+        <v>4176</v>
       </c>
     </row>
     <row r="19" spans="3:16" x14ac:dyDescent="0.35">
@@ -14895,7 +14898,7 @@
         <v>928</v>
       </c>
       <c r="J19" t="s">
-        <v>3290</v>
+        <v>3289</v>
       </c>
       <c r="K19" t="s">
         <v>455</v>
@@ -14904,7 +14907,7 @@
         <v>1109</v>
       </c>
       <c r="P19" t="s">
-        <v>4174</v>
+        <v>4177</v>
       </c>
     </row>
     <row r="20" spans="3:16" x14ac:dyDescent="0.35">
@@ -14927,7 +14930,7 @@
         <v>929</v>
       </c>
       <c r="J20" t="s">
-        <v>3291</v>
+        <v>3290</v>
       </c>
       <c r="K20" t="s">
         <v>45</v>
@@ -14936,7 +14939,7 @@
         <v>1023</v>
       </c>
       <c r="P20" t="s">
-        <v>4175</v>
+        <v>4178</v>
       </c>
     </row>
     <row r="21" spans="3:16" x14ac:dyDescent="0.35">
@@ -14959,7 +14962,7 @@
         <v>153</v>
       </c>
       <c r="J21" t="s">
-        <v>3292</v>
+        <v>3291</v>
       </c>
       <c r="K21" t="s">
         <v>16</v>
@@ -14968,7 +14971,7 @@
         <v>3569</v>
       </c>
       <c r="P21" t="s">
-        <v>4176</v>
+        <v>4179</v>
       </c>
     </row>
     <row r="22" spans="3:16" x14ac:dyDescent="0.35">
@@ -14991,7 +14994,7 @@
         <v>930</v>
       </c>
       <c r="J22" t="s">
-        <v>3293</v>
+        <v>3292</v>
       </c>
       <c r="K22" t="s">
         <v>3314</v>
@@ -15000,7 +15003,7 @@
         <v>3570</v>
       </c>
       <c r="P22" t="s">
-        <v>4177</v>
+        <v>4180</v>
       </c>
     </row>
     <row r="23" spans="3:16" x14ac:dyDescent="0.35">
@@ -15023,7 +15026,7 @@
         <v>46</v>
       </c>
       <c r="J23" t="s">
-        <v>3294</v>
+        <v>3293</v>
       </c>
       <c r="K23" t="s">
         <v>18</v>
@@ -15032,7 +15035,7 @@
         <v>3571</v>
       </c>
       <c r="P23" t="s">
-        <v>4178</v>
+        <v>4181</v>
       </c>
     </row>
     <row r="24" spans="3:16" x14ac:dyDescent="0.35">
@@ -15055,7 +15058,7 @@
         <v>931</v>
       </c>
       <c r="J24" t="s">
-        <v>3295</v>
+        <v>3294</v>
       </c>
       <c r="K24" t="s">
         <v>3315</v>
@@ -15064,7 +15067,7 @@
         <v>936</v>
       </c>
       <c r="P24" t="s">
-        <v>4179</v>
+        <v>4182</v>
       </c>
     </row>
     <row r="25" spans="3:16" x14ac:dyDescent="0.35">
@@ -15087,7 +15090,7 @@
         <v>932</v>
       </c>
       <c r="J25" t="s">
-        <v>134</v>
+        <v>3295</v>
       </c>
       <c r="K25" t="s">
         <v>3316</v>
@@ -15096,7 +15099,7 @@
         <v>3572</v>
       </c>
       <c r="P25" t="s">
-        <v>4180</v>
+        <v>4183</v>
       </c>
     </row>
     <row r="26" spans="3:16" x14ac:dyDescent="0.35">
@@ -15119,7 +15122,7 @@
         <v>933</v>
       </c>
       <c r="J26" t="s">
-        <v>66</v>
+        <v>134</v>
       </c>
       <c r="K26" t="s">
         <v>65</v>
@@ -15128,7 +15131,7 @@
         <v>3573</v>
       </c>
       <c r="P26" t="s">
-        <v>4181</v>
+        <v>4184</v>
       </c>
     </row>
     <row r="27" spans="3:16" x14ac:dyDescent="0.35">
@@ -15151,7 +15154,7 @@
         <v>934</v>
       </c>
       <c r="J27" t="s">
-        <v>3296</v>
+        <v>66</v>
       </c>
       <c r="K27" t="s">
         <v>86</v>
@@ -15160,7 +15163,7 @@
         <v>1135</v>
       </c>
       <c r="P27" t="s">
-        <v>4182</v>
+        <v>4185</v>
       </c>
     </row>
     <row r="28" spans="3:16" x14ac:dyDescent="0.35">
@@ -15183,7 +15186,7 @@
         <v>935</v>
       </c>
       <c r="J28" t="s">
-        <v>3297</v>
+        <v>3296</v>
       </c>
       <c r="K28" t="s">
         <v>3317</v>
@@ -15192,7 +15195,7 @@
         <v>3574</v>
       </c>
       <c r="P28" t="s">
-        <v>4183</v>
+        <v>4186</v>
       </c>
     </row>
     <row r="29" spans="3:16" x14ac:dyDescent="0.35">
@@ -15215,7 +15218,7 @@
         <v>936</v>
       </c>
       <c r="J29" t="s">
-        <v>3298</v>
+        <v>3297</v>
       </c>
       <c r="K29" t="s">
         <v>90</v>
@@ -15224,7 +15227,7 @@
         <v>3575</v>
       </c>
       <c r="P29" t="s">
-        <v>4184</v>
+        <v>4187</v>
       </c>
     </row>
     <row r="30" spans="3:16" x14ac:dyDescent="0.35">
@@ -15247,7 +15250,7 @@
         <v>937</v>
       </c>
       <c r="J30" t="s">
-        <v>3299</v>
+        <v>3298</v>
       </c>
       <c r="K30" t="s">
         <v>93</v>
@@ -15256,7 +15259,7 @@
         <v>1073</v>
       </c>
       <c r="P30" t="s">
-        <v>4185</v>
+        <v>4188</v>
       </c>
     </row>
     <row r="31" spans="3:16" x14ac:dyDescent="0.35">
@@ -15279,7 +15282,7 @@
         <v>938</v>
       </c>
       <c r="J31" t="s">
-        <v>3300</v>
+        <v>3299</v>
       </c>
       <c r="K31" t="s">
         <v>3318</v>
@@ -15288,7 +15291,7 @@
         <v>2760</v>
       </c>
       <c r="P31" t="s">
-        <v>4186</v>
+        <v>4189</v>
       </c>
     </row>
     <row r="32" spans="3:16" x14ac:dyDescent="0.35">
@@ -15311,7 +15314,7 @@
         <v>939</v>
       </c>
       <c r="J32" t="s">
-        <v>3301</v>
+        <v>3300</v>
       </c>
       <c r="K32" t="s">
         <v>22</v>
@@ -15320,7 +15323,7 @@
         <v>3576</v>
       </c>
       <c r="P32" t="s">
-        <v>4187</v>
+        <v>4190</v>
       </c>
     </row>
     <row r="33" spans="3:16" x14ac:dyDescent="0.35">
@@ -15343,7 +15346,7 @@
         <v>940</v>
       </c>
       <c r="J33" t="s">
-        <v>8</v>
+        <v>3301</v>
       </c>
       <c r="K33" t="s">
         <v>175</v>
@@ -15352,7 +15355,7 @@
         <v>3204</v>
       </c>
       <c r="P33" t="s">
-        <v>4188</v>
+        <v>4191</v>
       </c>
     </row>
     <row r="34" spans="3:16" x14ac:dyDescent="0.35">
@@ -15375,7 +15378,7 @@
         <v>941</v>
       </c>
       <c r="J34" t="s">
-        <v>3302</v>
+        <v>8</v>
       </c>
       <c r="K34" t="s">
         <v>105</v>
@@ -15384,7 +15387,7 @@
         <v>3577</v>
       </c>
       <c r="P34" t="s">
-        <v>4189</v>
+        <v>4192</v>
       </c>
     </row>
     <row r="35" spans="3:16" x14ac:dyDescent="0.35">
@@ -15404,7 +15407,7 @@
         <v>942</v>
       </c>
       <c r="J35" t="s">
-        <v>3303</v>
+        <v>3302</v>
       </c>
       <c r="K35" t="s">
         <v>3319</v>
@@ -15413,7 +15416,7 @@
         <v>384</v>
       </c>
       <c r="P35" t="s">
-        <v>4190</v>
+        <v>4193</v>
       </c>
     </row>
     <row r="36" spans="3:16" x14ac:dyDescent="0.35">
@@ -15433,7 +15436,7 @@
         <v>943</v>
       </c>
       <c r="J36" t="s">
-        <v>3304</v>
+        <v>3303</v>
       </c>
       <c r="K36" t="s">
         <v>3320</v>
@@ -15442,7 +15445,7 @@
         <v>3578</v>
       </c>
       <c r="P36" t="s">
-        <v>4191</v>
+        <v>4194</v>
       </c>
     </row>
     <row r="37" spans="3:16" x14ac:dyDescent="0.35">
@@ -15459,7 +15462,7 @@
         <v>944</v>
       </c>
       <c r="J37" t="s">
-        <v>2</v>
+        <v>3304</v>
       </c>
       <c r="K37" t="s">
         <v>51</v>
@@ -15468,7 +15471,7 @@
         <v>3579</v>
       </c>
       <c r="P37" t="s">
-        <v>4192</v>
+        <v>4195</v>
       </c>
     </row>
     <row r="38" spans="3:16" x14ac:dyDescent="0.35">
@@ -15482,7 +15485,7 @@
         <v>945</v>
       </c>
       <c r="J38" t="s">
-        <v>3305</v>
+        <v>2</v>
       </c>
       <c r="K38" t="s">
         <v>39</v>
@@ -15491,7 +15494,7 @@
         <v>3580</v>
       </c>
       <c r="P38" t="s">
-        <v>4193</v>
+        <v>4196</v>
       </c>
     </row>
     <row r="39" spans="3:16" x14ac:dyDescent="0.35">
@@ -15505,7 +15508,7 @@
         <v>946</v>
       </c>
       <c r="J39" t="s">
-        <v>2059</v>
+        <v>3305</v>
       </c>
       <c r="K39" t="s">
         <v>36</v>
@@ -15514,7 +15517,7 @@
         <v>3581</v>
       </c>
       <c r="P39" t="s">
-        <v>4194</v>
+        <v>4197</v>
       </c>
     </row>
     <row r="40" spans="3:16" x14ac:dyDescent="0.35">
@@ -15528,7 +15531,7 @@
         <v>947</v>
       </c>
       <c r="J40" t="s">
-        <v>59</v>
+        <v>2059</v>
       </c>
       <c r="K40" t="s">
         <v>113</v>
@@ -15537,7 +15540,7 @@
         <v>1238</v>
       </c>
       <c r="P40" t="s">
-        <v>4195</v>
+        <v>4198</v>
       </c>
     </row>
     <row r="41" spans="3:16" x14ac:dyDescent="0.35">
@@ -15551,7 +15554,7 @@
         <v>948</v>
       </c>
       <c r="J41" t="s">
-        <v>3306</v>
+        <v>59</v>
       </c>
       <c r="K41" t="s">
         <v>3321</v>
@@ -15560,7 +15563,7 @@
         <v>1251</v>
       </c>
       <c r="P41" t="s">
-        <v>4196</v>
+        <v>4199</v>
       </c>
     </row>
     <row r="42" spans="3:16" x14ac:dyDescent="0.35">
@@ -15574,7 +15577,7 @@
         <v>949</v>
       </c>
       <c r="J42" t="s">
-        <v>3307</v>
+        <v>3306</v>
       </c>
       <c r="K42" t="s">
         <v>3322</v>
@@ -15583,7 +15586,7 @@
         <v>1381</v>
       </c>
       <c r="P42" t="s">
-        <v>4197</v>
+        <v>4200</v>
       </c>
     </row>
     <row r="43" spans="3:16" x14ac:dyDescent="0.35">
@@ -15597,7 +15600,7 @@
         <v>950</v>
       </c>
       <c r="J43" t="s">
-        <v>3308</v>
+        <v>3307</v>
       </c>
       <c r="K43" t="s">
         <v>3323</v>
@@ -15606,7 +15609,7 @@
         <v>1559</v>
       </c>
       <c r="P43" t="s">
-        <v>4198</v>
+        <v>4201</v>
       </c>
     </row>
     <row r="44" spans="3:16" x14ac:dyDescent="0.35">
@@ -15620,7 +15623,7 @@
         <v>175</v>
       </c>
       <c r="J44" t="s">
-        <v>3309</v>
+        <v>3308</v>
       </c>
       <c r="K44" t="s">
         <v>3324</v>
@@ -15629,7 +15632,7 @@
         <v>3582</v>
       </c>
       <c r="P44" t="s">
-        <v>4199</v>
+        <v>4202</v>
       </c>
     </row>
     <row r="45" spans="3:16" x14ac:dyDescent="0.35">
@@ -15642,6 +15645,9 @@
       <c r="I45" t="s">
         <v>951</v>
       </c>
+      <c r="J45" t="s">
+        <v>3309</v>
+      </c>
       <c r="K45" t="s">
         <v>3325</v>
       </c>
@@ -15649,7 +15655,7 @@
         <v>1034</v>
       </c>
       <c r="P45" t="s">
-        <v>4200</v>
+        <v>4203</v>
       </c>
     </row>
     <row r="46" spans="3:16" x14ac:dyDescent="0.35">
@@ -15669,7 +15675,7 @@
         <v>3583</v>
       </c>
       <c r="P46" t="s">
-        <v>4201</v>
+        <v>4204</v>
       </c>
     </row>
     <row r="47" spans="3:16" x14ac:dyDescent="0.35">
@@ -15689,7 +15695,7 @@
         <v>1261</v>
       </c>
       <c r="P47" t="s">
-        <v>4202</v>
+        <v>4205</v>
       </c>
     </row>
     <row r="48" spans="3:16" x14ac:dyDescent="0.35">
@@ -15709,7 +15715,7 @@
         <v>1427</v>
       </c>
       <c r="P48" t="s">
-        <v>4203</v>
+        <v>4206</v>
       </c>
     </row>
     <row r="49" spans="6:16" x14ac:dyDescent="0.35">
@@ -15729,7 +15735,7 @@
         <v>1499</v>
       </c>
       <c r="P49" t="s">
-        <v>4204</v>
+        <v>4207</v>
       </c>
     </row>
     <row r="50" spans="6:16" x14ac:dyDescent="0.35">
@@ -15749,7 +15755,7 @@
         <v>33</v>
       </c>
       <c r="P50" t="s">
-        <v>4205</v>
+        <v>4208</v>
       </c>
     </row>
     <row r="51" spans="6:16" x14ac:dyDescent="0.35">
@@ -15769,7 +15775,7 @@
         <v>415</v>
       </c>
       <c r="P51" t="s">
-        <v>4206</v>
+        <v>4209</v>
       </c>
     </row>
     <row r="52" spans="6:16" x14ac:dyDescent="0.35">
@@ -15789,7 +15795,7 @@
         <v>3584</v>
       </c>
       <c r="P52" t="s">
-        <v>4207</v>
+        <v>4210</v>
       </c>
     </row>
     <row r="53" spans="6:16" x14ac:dyDescent="0.35">
@@ -15809,7 +15815,7 @@
         <v>2211</v>
       </c>
       <c r="P53" t="s">
-        <v>4208</v>
+        <v>4211</v>
       </c>
     </row>
     <row r="54" spans="6:16" x14ac:dyDescent="0.35">
@@ -15829,7 +15835,7 @@
         <v>3585</v>
       </c>
       <c r="P54" t="s">
-        <v>4209</v>
+        <v>4212</v>
       </c>
     </row>
     <row r="55" spans="6:16" x14ac:dyDescent="0.35">
@@ -15849,7 +15855,7 @@
         <v>3586</v>
       </c>
       <c r="P55" t="s">
-        <v>4210</v>
+        <v>4213</v>
       </c>
     </row>
     <row r="56" spans="6:16" x14ac:dyDescent="0.35">
@@ -15869,7 +15875,7 @@
         <v>3587</v>
       </c>
       <c r="P56" t="s">
-        <v>4211</v>
+        <v>4214</v>
       </c>
     </row>
     <row r="57" spans="6:16" x14ac:dyDescent="0.35">
@@ -15889,7 +15895,7 @@
         <v>3588</v>
       </c>
       <c r="P57" t="s">
-        <v>4212</v>
+        <v>4215</v>
       </c>
     </row>
     <row r="58" spans="6:16" x14ac:dyDescent="0.35">
@@ -15909,7 +15915,7 @@
         <v>3589</v>
       </c>
       <c r="P58" t="s">
-        <v>4213</v>
+        <v>4216</v>
       </c>
     </row>
     <row r="59" spans="6:16" x14ac:dyDescent="0.35">
@@ -15929,7 +15935,7 @@
         <v>3590</v>
       </c>
       <c r="P59" t="s">
-        <v>4214</v>
+        <v>4217</v>
       </c>
     </row>
     <row r="60" spans="6:16" x14ac:dyDescent="0.35">
@@ -15949,7 +15955,7 @@
         <v>1736</v>
       </c>
       <c r="P60" t="s">
-        <v>4215</v>
+        <v>4218</v>
       </c>
     </row>
     <row r="61" spans="6:16" x14ac:dyDescent="0.35">
@@ -15969,7 +15975,7 @@
         <v>3591</v>
       </c>
       <c r="P61" t="s">
-        <v>4216</v>
+        <v>4219</v>
       </c>
     </row>
     <row r="62" spans="6:16" x14ac:dyDescent="0.35">
@@ -15989,7 +15995,7 @@
         <v>2146</v>
       </c>
       <c r="P62" t="s">
-        <v>4217</v>
+        <v>4220</v>
       </c>
     </row>
     <row r="63" spans="6:16" x14ac:dyDescent="0.35">
@@ -16009,7 +16015,7 @@
         <v>3592</v>
       </c>
       <c r="P63" t="s">
-        <v>4218</v>
+        <v>4221</v>
       </c>
     </row>
     <row r="64" spans="6:16" x14ac:dyDescent="0.35">
@@ -16029,7 +16035,7 @@
         <v>3593</v>
       </c>
       <c r="P64" t="s">
-        <v>4219</v>
+        <v>4222</v>
       </c>
     </row>
     <row r="65" spans="6:16" x14ac:dyDescent="0.35">
@@ -16049,7 +16055,7 @@
         <v>3594</v>
       </c>
       <c r="P65" t="s">
-        <v>4220</v>
+        <v>4223</v>
       </c>
     </row>
     <row r="66" spans="6:16" x14ac:dyDescent="0.35">
@@ -16069,7 +16075,7 @@
         <v>1234</v>
       </c>
       <c r="P66" t="s">
-        <v>4221</v>
+        <v>4224</v>
       </c>
     </row>
     <row r="67" spans="6:16" x14ac:dyDescent="0.35">
@@ -16089,7 +16095,7 @@
         <v>3595</v>
       </c>
       <c r="P67" t="s">
-        <v>4222</v>
+        <v>4225</v>
       </c>
     </row>
     <row r="68" spans="6:16" x14ac:dyDescent="0.35">
@@ -16109,7 +16115,7 @@
         <v>996</v>
       </c>
       <c r="P68" t="s">
-        <v>4223</v>
+        <v>4226</v>
       </c>
     </row>
     <row r="69" spans="6:16" x14ac:dyDescent="0.35">
@@ -16129,7 +16135,7 @@
         <v>1579</v>
       </c>
       <c r="P69" t="s">
-        <v>4224</v>
+        <v>4227</v>
       </c>
     </row>
     <row r="70" spans="6:16" x14ac:dyDescent="0.35">
@@ -16149,7 +16155,7 @@
         <v>3596</v>
       </c>
       <c r="P70" t="s">
-        <v>4225</v>
+        <v>4228</v>
       </c>
     </row>
     <row r="71" spans="6:16" x14ac:dyDescent="0.35">
@@ -16169,7 +16175,7 @@
         <v>2009</v>
       </c>
       <c r="P71" t="s">
-        <v>4226</v>
+        <v>4229</v>
       </c>
     </row>
     <row r="72" spans="6:16" x14ac:dyDescent="0.35">
@@ -16189,7 +16195,7 @@
         <v>3597</v>
       </c>
       <c r="P72" t="s">
-        <v>4227</v>
+        <v>4230</v>
       </c>
     </row>
     <row r="73" spans="6:16" x14ac:dyDescent="0.35">
@@ -16209,7 +16215,7 @@
         <v>1971</v>
       </c>
       <c r="P73" t="s">
-        <v>4228</v>
+        <v>4231</v>
       </c>
     </row>
     <row r="74" spans="6:16" x14ac:dyDescent="0.35">
@@ -16229,7 +16235,7 @@
         <v>3598</v>
       </c>
       <c r="P74" t="s">
-        <v>4229</v>
+        <v>4232</v>
       </c>
     </row>
     <row r="75" spans="6:16" x14ac:dyDescent="0.35">
@@ -16249,7 +16255,7 @@
         <v>3599</v>
       </c>
       <c r="P75" t="s">
-        <v>4230</v>
+        <v>4233</v>
       </c>
     </row>
     <row r="76" spans="6:16" x14ac:dyDescent="0.35">
@@ -16269,7 +16275,7 @@
         <v>3600</v>
       </c>
       <c r="P76" t="s">
-        <v>4231</v>
+        <v>4234</v>
       </c>
     </row>
     <row r="77" spans="6:16" x14ac:dyDescent="0.35">
@@ -16289,7 +16295,7 @@
         <v>3601</v>
       </c>
       <c r="P77" t="s">
-        <v>4232</v>
+        <v>4235</v>
       </c>
     </row>
     <row r="78" spans="6:16" x14ac:dyDescent="0.35">
@@ -16309,7 +16315,7 @@
         <v>3602</v>
       </c>
       <c r="P78" t="s">
-        <v>4233</v>
+        <v>4236</v>
       </c>
     </row>
     <row r="79" spans="6:16" x14ac:dyDescent="0.35">
@@ -16329,7 +16335,7 @@
         <v>3603</v>
       </c>
       <c r="P79" t="s">
-        <v>4234</v>
+        <v>4237</v>
       </c>
     </row>
     <row r="80" spans="6:16" x14ac:dyDescent="0.35">
@@ -16349,7 +16355,7 @@
         <v>3604</v>
       </c>
       <c r="P80" t="s">
-        <v>4235</v>
+        <v>4238</v>
       </c>
     </row>
     <row r="81" spans="6:16" x14ac:dyDescent="0.35">
@@ -16369,7 +16375,7 @@
         <v>203</v>
       </c>
       <c r="P81" t="s">
-        <v>4236</v>
+        <v>4239</v>
       </c>
     </row>
     <row r="82" spans="6:16" x14ac:dyDescent="0.35">
@@ -16389,7 +16395,7 @@
         <v>1881</v>
       </c>
       <c r="P82" t="s">
-        <v>4237</v>
+        <v>4240</v>
       </c>
     </row>
     <row r="83" spans="6:16" x14ac:dyDescent="0.35">
@@ -16409,7 +16415,7 @@
         <v>2455</v>
       </c>
       <c r="P83" t="s">
-        <v>4238</v>
+        <v>4241</v>
       </c>
     </row>
     <row r="84" spans="6:16" x14ac:dyDescent="0.35">
@@ -16429,7 +16435,7 @@
         <v>1818</v>
       </c>
       <c r="P84" t="s">
-        <v>4239</v>
+        <v>4242</v>
       </c>
     </row>
     <row r="85" spans="6:16" x14ac:dyDescent="0.35">
@@ -16449,7 +16455,7 @@
         <v>3605</v>
       </c>
       <c r="P85" t="s">
-        <v>4240</v>
+        <v>4243</v>
       </c>
     </row>
     <row r="86" spans="6:16" x14ac:dyDescent="0.35">
@@ -16469,7 +16475,7 @@
         <v>1096</v>
       </c>
       <c r="P86" t="s">
-        <v>4241</v>
+        <v>4244</v>
       </c>
     </row>
     <row r="87" spans="6:16" x14ac:dyDescent="0.35">
@@ -16489,7 +16495,7 @@
         <v>3606</v>
       </c>
       <c r="P87" t="s">
-        <v>4242</v>
+        <v>4245</v>
       </c>
     </row>
     <row r="88" spans="6:16" x14ac:dyDescent="0.35">
@@ -16509,7 +16515,7 @@
         <v>3607</v>
       </c>
       <c r="P88" t="s">
-        <v>4243</v>
+        <v>4246</v>
       </c>
     </row>
     <row r="89" spans="6:16" x14ac:dyDescent="0.35">
@@ -16529,7 +16535,7 @@
         <v>3608</v>
       </c>
       <c r="P89" t="s">
-        <v>4244</v>
+        <v>4247</v>
       </c>
     </row>
     <row r="90" spans="6:16" x14ac:dyDescent="0.35">
@@ -16546,7 +16552,7 @@
         <v>3609</v>
       </c>
       <c r="P90" t="s">
-        <v>4245</v>
+        <v>4248</v>
       </c>
     </row>
     <row r="91" spans="6:16" x14ac:dyDescent="0.35">
@@ -16563,7 +16569,7 @@
         <v>3610</v>
       </c>
       <c r="P91" t="s">
-        <v>4246</v>
+        <v>4249</v>
       </c>
     </row>
     <row r="92" spans="6:16" x14ac:dyDescent="0.35">
@@ -16580,7 +16586,7 @@
         <v>3611</v>
       </c>
       <c r="P92" t="s">
-        <v>4247</v>
+        <v>4250</v>
       </c>
     </row>
     <row r="93" spans="6:16" x14ac:dyDescent="0.35">
@@ -16597,7 +16603,7 @@
         <v>3612</v>
       </c>
       <c r="P93" t="s">
-        <v>4248</v>
+        <v>4251</v>
       </c>
     </row>
     <row r="94" spans="6:16" x14ac:dyDescent="0.35">
@@ -16614,7 +16620,7 @@
         <v>3613</v>
       </c>
       <c r="P94" t="s">
-        <v>4249</v>
+        <v>4252</v>
       </c>
     </row>
     <row r="95" spans="6:16" x14ac:dyDescent="0.35">
@@ -16631,7 +16637,7 @@
         <v>3614</v>
       </c>
       <c r="P95" t="s">
-        <v>4250</v>
+        <v>4253</v>
       </c>
     </row>
     <row r="96" spans="6:16" x14ac:dyDescent="0.35">
@@ -16648,7 +16654,7 @@
         <v>2994</v>
       </c>
       <c r="P96" t="s">
-        <v>4251</v>
+        <v>4254</v>
       </c>
     </row>
     <row r="97" spans="7:16" x14ac:dyDescent="0.35">
@@ -16665,7 +16671,7 @@
         <v>1299</v>
       </c>
       <c r="P97" t="s">
-        <v>4252</v>
+        <v>4255</v>
       </c>
     </row>
     <row r="98" spans="7:16" x14ac:dyDescent="0.35">
@@ -16682,7 +16688,7 @@
         <v>1540</v>
       </c>
       <c r="P98" t="s">
-        <v>4253</v>
+        <v>4256</v>
       </c>
     </row>
     <row r="99" spans="7:16" x14ac:dyDescent="0.35">
@@ -16699,7 +16705,7 @@
         <v>2557</v>
       </c>
       <c r="P99" t="s">
-        <v>4254</v>
+        <v>4257</v>
       </c>
     </row>
     <row r="100" spans="7:16" x14ac:dyDescent="0.35">
@@ -16716,7 +16722,7 @@
         <v>3615</v>
       </c>
       <c r="P100" t="s">
-        <v>4255</v>
+        <v>4258</v>
       </c>
     </row>
     <row r="101" spans="7:16" x14ac:dyDescent="0.35">
@@ -16733,7 +16739,7 @@
         <v>3616</v>
       </c>
       <c r="P101" t="s">
-        <v>4256</v>
+        <v>4259</v>
       </c>
     </row>
     <row r="102" spans="7:16" x14ac:dyDescent="0.35">
@@ -16750,7 +16756,7 @@
         <v>3617</v>
       </c>
       <c r="P102" t="s">
-        <v>4257</v>
+        <v>4260</v>
       </c>
     </row>
     <row r="103" spans="7:16" x14ac:dyDescent="0.35">
@@ -16767,7 +16773,7 @@
         <v>3618</v>
       </c>
       <c r="P103" t="s">
-        <v>4258</v>
+        <v>4261</v>
       </c>
     </row>
     <row r="104" spans="7:16" x14ac:dyDescent="0.35">
@@ -16784,7 +16790,7 @@
         <v>3619</v>
       </c>
       <c r="P104" t="s">
-        <v>4259</v>
+        <v>4262</v>
       </c>
     </row>
     <row r="105" spans="7:16" x14ac:dyDescent="0.35">
@@ -16801,7 +16807,7 @@
         <v>3620</v>
       </c>
       <c r="P105" t="s">
-        <v>4260</v>
+        <v>4263</v>
       </c>
     </row>
     <row r="106" spans="7:16" x14ac:dyDescent="0.35">
@@ -16818,7 +16824,7 @@
         <v>1041</v>
       </c>
       <c r="P106" t="s">
-        <v>4261</v>
+        <v>4264</v>
       </c>
     </row>
     <row r="107" spans="7:16" x14ac:dyDescent="0.35">
@@ -16835,7 +16841,7 @@
         <v>3621</v>
       </c>
       <c r="P107" t="s">
-        <v>4262</v>
+        <v>4265</v>
       </c>
     </row>
     <row r="108" spans="7:16" x14ac:dyDescent="0.35">
@@ -16852,7 +16858,7 @@
         <v>3622</v>
       </c>
       <c r="P108" t="s">
-        <v>4263</v>
+        <v>4266</v>
       </c>
     </row>
     <row r="109" spans="7:16" x14ac:dyDescent="0.35">
@@ -16869,7 +16875,7 @@
         <v>1420</v>
       </c>
       <c r="P109" t="s">
-        <v>4264</v>
+        <v>4267</v>
       </c>
     </row>
     <row r="110" spans="7:16" x14ac:dyDescent="0.35">
@@ -16886,7 +16892,7 @@
         <v>3623</v>
       </c>
       <c r="P110" t="s">
-        <v>4265</v>
+        <v>4268</v>
       </c>
     </row>
     <row r="111" spans="7:16" x14ac:dyDescent="0.35">
@@ -16903,7 +16909,7 @@
         <v>1370</v>
       </c>
       <c r="P111" t="s">
-        <v>4266</v>
+        <v>4269</v>
       </c>
     </row>
     <row r="112" spans="7:16" x14ac:dyDescent="0.35">
@@ -16920,7 +16926,7 @@
         <v>3624</v>
       </c>
       <c r="P112" t="s">
-        <v>4267</v>
+        <v>4270</v>
       </c>
     </row>
     <row r="113" spans="7:16" x14ac:dyDescent="0.35">
@@ -16937,7 +16943,7 @@
         <v>3625</v>
       </c>
       <c r="P113" t="s">
-        <v>4268</v>
+        <v>4271</v>
       </c>
     </row>
     <row r="114" spans="7:16" x14ac:dyDescent="0.35">
@@ -16954,7 +16960,7 @@
         <v>1518</v>
       </c>
       <c r="P114" t="s">
-        <v>4269</v>
+        <v>4272</v>
       </c>
     </row>
     <row r="115" spans="7:16" x14ac:dyDescent="0.35">
@@ -16971,7 +16977,7 @@
         <v>1339</v>
       </c>
       <c r="P115" t="s">
-        <v>4270</v>
+        <v>4273</v>
       </c>
     </row>
     <row r="116" spans="7:16" x14ac:dyDescent="0.35">
@@ -16988,7 +16994,7 @@
         <v>3626</v>
       </c>
       <c r="P116" t="s">
-        <v>4271</v>
+        <v>4274</v>
       </c>
     </row>
     <row r="117" spans="7:16" x14ac:dyDescent="0.35">
@@ -17005,7 +17011,7 @@
         <v>3627</v>
       </c>
       <c r="P117" t="s">
-        <v>4272</v>
+        <v>4275</v>
       </c>
     </row>
     <row r="118" spans="7:16" x14ac:dyDescent="0.35">
@@ -17022,7 +17028,7 @@
         <v>3628</v>
       </c>
       <c r="P118" t="s">
-        <v>4273</v>
+        <v>4276</v>
       </c>
     </row>
     <row r="119" spans="7:16" x14ac:dyDescent="0.35">
@@ -17039,7 +17045,7 @@
         <v>3629</v>
       </c>
       <c r="P119" t="s">
-        <v>4274</v>
+        <v>4277</v>
       </c>
     </row>
     <row r="120" spans="7:16" x14ac:dyDescent="0.35">
@@ -17056,7 +17062,7 @@
         <v>3630</v>
       </c>
       <c r="P120" t="s">
-        <v>4275</v>
+        <v>4278</v>
       </c>
     </row>
     <row r="121" spans="7:16" x14ac:dyDescent="0.35">
@@ -17073,7 +17079,7 @@
         <v>3631</v>
       </c>
       <c r="P121" t="s">
-        <v>4276</v>
+        <v>4279</v>
       </c>
     </row>
     <row r="122" spans="7:16" x14ac:dyDescent="0.35">
@@ -17090,7 +17096,7 @@
         <v>1097</v>
       </c>
       <c r="P122" t="s">
-        <v>4277</v>
+        <v>4280</v>
       </c>
     </row>
     <row r="123" spans="7:16" x14ac:dyDescent="0.35">
@@ -17107,7 +17113,7 @@
         <v>969</v>
       </c>
       <c r="P123" t="s">
-        <v>4278</v>
+        <v>4281</v>
       </c>
     </row>
     <row r="124" spans="7:16" x14ac:dyDescent="0.35">
@@ -17124,7 +17130,7 @@
         <v>1883</v>
       </c>
       <c r="P124" t="s">
-        <v>4279</v>
+        <v>4282</v>
       </c>
     </row>
     <row r="125" spans="7:16" x14ac:dyDescent="0.35">
@@ -17141,7 +17147,7 @@
         <v>1259</v>
       </c>
       <c r="P125" t="s">
-        <v>4280</v>
+        <v>4283</v>
       </c>
     </row>
     <row r="126" spans="7:16" x14ac:dyDescent="0.35">
@@ -17158,7 +17164,7 @@
         <v>3632</v>
       </c>
       <c r="P126" t="s">
-        <v>4281</v>
+        <v>4284</v>
       </c>
     </row>
     <row r="127" spans="7:16" x14ac:dyDescent="0.35">
@@ -17175,7 +17181,7 @@
         <v>3633</v>
       </c>
       <c r="P127" t="s">
-        <v>4282</v>
+        <v>4285</v>
       </c>
     </row>
     <row r="128" spans="7:16" x14ac:dyDescent="0.35">
@@ -17192,7 +17198,7 @@
         <v>3634</v>
       </c>
       <c r="P128" t="s">
-        <v>4283</v>
+        <v>4286</v>
       </c>
     </row>
     <row r="129" spans="7:16" x14ac:dyDescent="0.35">
@@ -17209,7 +17215,7 @@
         <v>985</v>
       </c>
       <c r="P129" t="s">
-        <v>4284</v>
+        <v>4287</v>
       </c>
     </row>
     <row r="130" spans="7:16" x14ac:dyDescent="0.35">
@@ -17226,7 +17232,7 @@
         <v>1609</v>
       </c>
       <c r="P130" t="s">
-        <v>4285</v>
+        <v>4288</v>
       </c>
     </row>
     <row r="131" spans="7:16" x14ac:dyDescent="0.35">
@@ -17243,7 +17249,7 @@
         <v>3635</v>
       </c>
       <c r="P131" t="s">
-        <v>4286</v>
+        <v>4289</v>
       </c>
     </row>
     <row r="132" spans="7:16" x14ac:dyDescent="0.35">
@@ -17260,7 +17266,7 @@
         <v>2911</v>
       </c>
       <c r="P132" t="s">
-        <v>4287</v>
+        <v>4290</v>
       </c>
     </row>
     <row r="133" spans="7:16" x14ac:dyDescent="0.35">
@@ -17277,7 +17283,7 @@
         <v>3636</v>
       </c>
       <c r="P133" t="s">
-        <v>4288</v>
+        <v>4291</v>
       </c>
     </row>
     <row r="134" spans="7:16" x14ac:dyDescent="0.35">
@@ -17294,7 +17300,7 @@
         <v>3637</v>
       </c>
       <c r="P134" t="s">
-        <v>4289</v>
+        <v>4292</v>
       </c>
     </row>
     <row r="135" spans="7:16" x14ac:dyDescent="0.35">
@@ -17311,7 +17317,7 @@
         <v>1296</v>
       </c>
       <c r="P135" t="s">
-        <v>4290</v>
+        <v>4293</v>
       </c>
     </row>
     <row r="136" spans="7:16" x14ac:dyDescent="0.35">
@@ -17328,7 +17334,7 @@
         <v>940</v>
       </c>
       <c r="P136" t="s">
-        <v>4291</v>
+        <v>4294</v>
       </c>
     </row>
     <row r="137" spans="7:16" x14ac:dyDescent="0.35">
@@ -17345,7 +17351,7 @@
         <v>3638</v>
       </c>
       <c r="P137" t="s">
-        <v>4292</v>
+        <v>4295</v>
       </c>
     </row>
     <row r="138" spans="7:16" x14ac:dyDescent="0.35">
@@ -17362,7 +17368,7 @@
         <v>3639</v>
       </c>
       <c r="P138" t="s">
-        <v>4293</v>
+        <v>4296</v>
       </c>
     </row>
     <row r="139" spans="7:16" x14ac:dyDescent="0.35">
@@ -17379,7 +17385,7 @@
         <v>930</v>
       </c>
       <c r="P139" t="s">
-        <v>4294</v>
+        <v>4297</v>
       </c>
     </row>
     <row r="140" spans="7:16" x14ac:dyDescent="0.35">
@@ -17396,7 +17402,7 @@
         <v>238</v>
       </c>
       <c r="P140" t="s">
-        <v>4295</v>
+        <v>4298</v>
       </c>
     </row>
     <row r="141" spans="7:16" x14ac:dyDescent="0.35">
@@ -17413,7 +17419,7 @@
         <v>3640</v>
       </c>
       <c r="P141" t="s">
-        <v>4296</v>
+        <v>4299</v>
       </c>
     </row>
     <row r="142" spans="7:16" x14ac:dyDescent="0.35">
@@ -17430,7 +17436,7 @@
         <v>1433</v>
       </c>
       <c r="P142" t="s">
-        <v>4297</v>
+        <v>4300</v>
       </c>
     </row>
     <row r="143" spans="7:16" x14ac:dyDescent="0.35">
@@ -17447,7 +17453,7 @@
         <v>3641</v>
       </c>
       <c r="P143" t="s">
-        <v>4298</v>
+        <v>4301</v>
       </c>
     </row>
     <row r="144" spans="7:16" x14ac:dyDescent="0.35">
@@ -17464,7 +17470,7 @@
         <v>1205</v>
       </c>
       <c r="P144" t="s">
-        <v>4299</v>
+        <v>4302</v>
       </c>
     </row>
     <row r="145" spans="7:16" x14ac:dyDescent="0.35">
@@ -17481,7 +17487,7 @@
         <v>1577</v>
       </c>
       <c r="P145" t="s">
-        <v>4300</v>
+        <v>4303</v>
       </c>
     </row>
     <row r="146" spans="7:16" x14ac:dyDescent="0.35">
@@ -17498,7 +17504,7 @@
         <v>3642</v>
       </c>
       <c r="P146" t="s">
-        <v>4301</v>
+        <v>4304</v>
       </c>
     </row>
     <row r="147" spans="7:16" x14ac:dyDescent="0.35">
@@ -17515,7 +17521,7 @@
         <v>3643</v>
       </c>
       <c r="P147" t="s">
-        <v>4302</v>
+        <v>4305</v>
       </c>
     </row>
     <row r="148" spans="7:16" x14ac:dyDescent="0.35">
@@ -17532,7 +17538,7 @@
         <v>3644</v>
       </c>
       <c r="P148" t="s">
-        <v>4303</v>
+        <v>4306</v>
       </c>
     </row>
     <row r="149" spans="7:16" x14ac:dyDescent="0.35">
@@ -17549,7 +17555,7 @@
         <v>1513</v>
       </c>
       <c r="P149" t="s">
-        <v>4304</v>
+        <v>4307</v>
       </c>
     </row>
     <row r="150" spans="7:16" x14ac:dyDescent="0.35">
@@ -17566,7 +17572,7 @@
         <v>2060</v>
       </c>
       <c r="P150" t="s">
-        <v>4305</v>
+        <v>4308</v>
       </c>
     </row>
     <row r="151" spans="7:16" x14ac:dyDescent="0.35">
@@ -17583,7 +17589,7 @@
         <v>1017</v>
       </c>
       <c r="P151" t="s">
-        <v>4306</v>
+        <v>4309</v>
       </c>
     </row>
     <row r="152" spans="7:16" x14ac:dyDescent="0.35">
@@ -17600,7 +17606,7 @@
         <v>3645</v>
       </c>
       <c r="P152" t="s">
-        <v>4307</v>
+        <v>4310</v>
       </c>
     </row>
     <row r="153" spans="7:16" x14ac:dyDescent="0.35">
@@ -17617,7 +17623,7 @@
         <v>3646</v>
       </c>
       <c r="P153" t="s">
-        <v>4308</v>
+        <v>4311</v>
       </c>
     </row>
     <row r="154" spans="7:16" x14ac:dyDescent="0.35">
@@ -17634,7 +17640,7 @@
         <v>1236</v>
       </c>
       <c r="P154" t="s">
-        <v>4309</v>
+        <v>4312</v>
       </c>
     </row>
     <row r="155" spans="7:16" x14ac:dyDescent="0.35">
@@ -17651,7 +17657,7 @@
         <v>3647</v>
       </c>
       <c r="P155" t="s">
-        <v>4310</v>
+        <v>4313</v>
       </c>
     </row>
     <row r="156" spans="7:16" x14ac:dyDescent="0.35">
@@ -17668,7 +17674,7 @@
         <v>1450</v>
       </c>
       <c r="P156" t="s">
-        <v>4311</v>
+        <v>4314</v>
       </c>
     </row>
     <row r="157" spans="7:16" x14ac:dyDescent="0.35">
@@ -17685,7 +17691,7 @@
         <v>1766</v>
       </c>
       <c r="P157" t="s">
-        <v>4312</v>
+        <v>4315</v>
       </c>
     </row>
     <row r="158" spans="7:16" x14ac:dyDescent="0.35">
@@ -17702,7 +17708,7 @@
         <v>3648</v>
       </c>
       <c r="P158" t="s">
-        <v>4313</v>
+        <v>4316</v>
       </c>
     </row>
     <row r="159" spans="7:16" x14ac:dyDescent="0.35">
@@ -17719,7 +17725,7 @@
         <v>3649</v>
       </c>
       <c r="P159" t="s">
-        <v>4314</v>
+        <v>4317</v>
       </c>
     </row>
     <row r="160" spans="7:16" x14ac:dyDescent="0.35">
@@ -17736,7 +17742,7 @@
         <v>3650</v>
       </c>
       <c r="P160" t="s">
-        <v>4315</v>
+        <v>4318</v>
       </c>
     </row>
     <row r="161" spans="7:16" x14ac:dyDescent="0.35">
@@ -17753,7 +17759,7 @@
         <v>2199</v>
       </c>
       <c r="P161" t="s">
-        <v>4316</v>
+        <v>4319</v>
       </c>
     </row>
     <row r="162" spans="7:16" x14ac:dyDescent="0.35">
@@ -17770,7 +17776,7 @@
         <v>3651</v>
       </c>
       <c r="P162" t="s">
-        <v>4317</v>
+        <v>4320</v>
       </c>
     </row>
     <row r="163" spans="7:16" x14ac:dyDescent="0.35">
@@ -17787,7 +17793,7 @@
         <v>3652</v>
       </c>
       <c r="P163" t="s">
-        <v>4318</v>
+        <v>4321</v>
       </c>
     </row>
     <row r="164" spans="7:16" x14ac:dyDescent="0.35">
@@ -17804,7 +17810,7 @@
         <v>3653</v>
       </c>
       <c r="P164" t="s">
-        <v>4319</v>
+        <v>4322</v>
       </c>
     </row>
     <row r="165" spans="7:16" x14ac:dyDescent="0.35">
@@ -17821,7 +17827,7 @@
         <v>3654</v>
       </c>
       <c r="P165" t="s">
-        <v>4320</v>
+        <v>4323</v>
       </c>
     </row>
     <row r="166" spans="7:16" x14ac:dyDescent="0.35">
@@ -17838,7 +17844,7 @@
         <v>3655</v>
       </c>
       <c r="P166" t="s">
-        <v>4321</v>
+        <v>4324</v>
       </c>
     </row>
     <row r="167" spans="7:16" x14ac:dyDescent="0.35">
@@ -17855,7 +17861,7 @@
         <v>3656</v>
       </c>
       <c r="P167" t="s">
-        <v>4322</v>
+        <v>4325</v>
       </c>
     </row>
     <row r="168" spans="7:16" x14ac:dyDescent="0.35">
@@ -17872,7 +17878,7 @@
         <v>3657</v>
       </c>
       <c r="P168" t="s">
-        <v>4323</v>
+        <v>4326</v>
       </c>
     </row>
     <row r="169" spans="7:16" x14ac:dyDescent="0.35">
@@ -17889,7 +17895,7 @@
         <v>3658</v>
       </c>
       <c r="P169" t="s">
-        <v>4324</v>
+        <v>4327</v>
       </c>
     </row>
     <row r="170" spans="7:16" x14ac:dyDescent="0.35">
@@ -17906,7 +17912,7 @@
         <v>2100</v>
       </c>
       <c r="P170" t="s">
-        <v>4325</v>
+        <v>4328</v>
       </c>
     </row>
     <row r="171" spans="7:16" x14ac:dyDescent="0.35">
@@ -17923,7 +17929,7 @@
         <v>3659</v>
       </c>
       <c r="P171" t="s">
-        <v>4326</v>
+        <v>4329</v>
       </c>
     </row>
     <row r="172" spans="7:16" x14ac:dyDescent="0.35">
@@ -17940,7 +17946,7 @@
         <v>3660</v>
       </c>
       <c r="P172" t="s">
-        <v>4327</v>
+        <v>4330</v>
       </c>
     </row>
     <row r="173" spans="7:16" x14ac:dyDescent="0.35">
@@ -17957,7 +17963,7 @@
         <v>3661</v>
       </c>
       <c r="P173" t="s">
-        <v>4328</v>
+        <v>4331</v>
       </c>
     </row>
     <row r="174" spans="7:16" x14ac:dyDescent="0.35">
@@ -17974,7 +17980,7 @@
         <v>975</v>
       </c>
       <c r="P174" t="s">
-        <v>4329</v>
+        <v>4332</v>
       </c>
     </row>
     <row r="175" spans="7:16" x14ac:dyDescent="0.35">
@@ -17991,7 +17997,7 @@
         <v>299</v>
       </c>
       <c r="P175" t="s">
-        <v>4330</v>
+        <v>4333</v>
       </c>
     </row>
     <row r="176" spans="7:16" x14ac:dyDescent="0.35">
@@ -18008,7 +18014,7 @@
         <v>1186</v>
       </c>
       <c r="P176" t="s">
-        <v>4331</v>
+        <v>4334</v>
       </c>
     </row>
     <row r="177" spans="7:16" x14ac:dyDescent="0.35">
@@ -18025,7 +18031,7 @@
         <v>3662</v>
       </c>
       <c r="P177" t="s">
-        <v>4332</v>
+        <v>4335</v>
       </c>
     </row>
     <row r="178" spans="7:16" x14ac:dyDescent="0.35">
@@ -18042,7 +18048,7 @@
         <v>3663</v>
       </c>
       <c r="P178" t="s">
-        <v>4333</v>
+        <v>4336</v>
       </c>
     </row>
     <row r="179" spans="7:16" x14ac:dyDescent="0.35">
@@ -18059,7 +18065,7 @@
         <v>1366</v>
       </c>
       <c r="P179" t="s">
-        <v>4334</v>
+        <v>4337</v>
       </c>
     </row>
     <row r="180" spans="7:16" x14ac:dyDescent="0.35">
@@ -18076,7 +18082,7 @@
         <v>923</v>
       </c>
       <c r="P180" t="s">
-        <v>4335</v>
+        <v>4338</v>
       </c>
     </row>
     <row r="181" spans="7:16" x14ac:dyDescent="0.35">
@@ -18093,7 +18099,7 @@
         <v>1006</v>
       </c>
       <c r="P181" t="s">
-        <v>4336</v>
+        <v>4339</v>
       </c>
     </row>
     <row r="182" spans="7:16" x14ac:dyDescent="0.35">
@@ -18110,7 +18116,7 @@
         <v>1735</v>
       </c>
       <c r="P182" t="s">
-        <v>4337</v>
+        <v>4340</v>
       </c>
     </row>
     <row r="183" spans="7:16" x14ac:dyDescent="0.35">
@@ -18127,7 +18133,7 @@
         <v>2584</v>
       </c>
       <c r="P183" t="s">
-        <v>4338</v>
+        <v>4341</v>
       </c>
     </row>
     <row r="184" spans="7:16" x14ac:dyDescent="0.35">
@@ -18144,7 +18150,7 @@
         <v>3664</v>
       </c>
       <c r="P184" t="s">
-        <v>4339</v>
+        <v>4342</v>
       </c>
     </row>
     <row r="185" spans="7:16" x14ac:dyDescent="0.35">
@@ -18161,7 +18167,7 @@
         <v>951</v>
       </c>
       <c r="P185" t="s">
-        <v>4340</v>
+        <v>4343</v>
       </c>
     </row>
     <row r="186" spans="7:16" x14ac:dyDescent="0.35">
@@ -18178,7 +18184,7 @@
         <v>3665</v>
       </c>
       <c r="P186" t="s">
-        <v>4341</v>
+        <v>4344</v>
       </c>
     </row>
     <row r="187" spans="7:16" x14ac:dyDescent="0.35">
@@ -18195,7 +18201,7 @@
         <v>3666</v>
       </c>
       <c r="P187" t="s">
-        <v>4342</v>
+        <v>4345</v>
       </c>
     </row>
     <row r="188" spans="7:16" x14ac:dyDescent="0.35">
@@ -18212,7 +18218,7 @@
         <v>1222</v>
       </c>
       <c r="P188" t="s">
-        <v>4343</v>
+        <v>4346</v>
       </c>
     </row>
     <row r="189" spans="7:16" x14ac:dyDescent="0.35">
@@ -18229,7 +18235,7 @@
         <v>3667</v>
       </c>
       <c r="P189" t="s">
-        <v>4344</v>
+        <v>4347</v>
       </c>
     </row>
     <row r="190" spans="7:16" x14ac:dyDescent="0.35">
@@ -18246,7 +18252,7 @@
         <v>1476</v>
       </c>
       <c r="P190" t="s">
-        <v>4345</v>
+        <v>4348</v>
       </c>
     </row>
     <row r="191" spans="7:16" x14ac:dyDescent="0.35">
@@ -18263,7 +18269,7 @@
         <v>3668</v>
       </c>
       <c r="P191" t="s">
-        <v>4346</v>
+        <v>4349</v>
       </c>
     </row>
     <row r="192" spans="7:16" x14ac:dyDescent="0.35">
@@ -18280,7 +18286,7 @@
         <v>1160</v>
       </c>
       <c r="P192" t="s">
-        <v>4347</v>
+        <v>4350</v>
       </c>
     </row>
     <row r="193" spans="7:16" x14ac:dyDescent="0.35">
@@ -18297,7 +18303,7 @@
         <v>3669</v>
       </c>
       <c r="P193" t="s">
-        <v>4348</v>
+        <v>4351</v>
       </c>
     </row>
     <row r="194" spans="7:16" x14ac:dyDescent="0.35">
@@ -18314,7 +18320,7 @@
         <v>1064</v>
       </c>
       <c r="P194" t="s">
-        <v>4349</v>
+        <v>4352</v>
       </c>
     </row>
     <row r="195" spans="7:16" x14ac:dyDescent="0.35">
@@ -18331,7 +18337,7 @@
         <v>3670</v>
       </c>
       <c r="P195" t="s">
-        <v>4350</v>
+        <v>4353</v>
       </c>
     </row>
     <row r="196" spans="7:16" x14ac:dyDescent="0.35">
@@ -18348,7 +18354,7 @@
         <v>1527</v>
       </c>
       <c r="P196" t="s">
-        <v>4351</v>
+        <v>4354</v>
       </c>
     </row>
     <row r="197" spans="7:16" x14ac:dyDescent="0.35">
@@ -18365,7 +18371,7 @@
         <v>1026</v>
       </c>
       <c r="P197" t="s">
-        <v>4352</v>
+        <v>4355</v>
       </c>
     </row>
     <row r="198" spans="7:16" x14ac:dyDescent="0.35">
@@ -18382,7 +18388,7 @@
         <v>3671</v>
       </c>
       <c r="P198" t="s">
-        <v>4353</v>
+        <v>4356</v>
       </c>
     </row>
     <row r="199" spans="7:16" x14ac:dyDescent="0.35">
@@ -18399,7 +18405,7 @@
         <v>3672</v>
       </c>
       <c r="P199" t="s">
-        <v>4354</v>
+        <v>4357</v>
       </c>
     </row>
     <row r="200" spans="7:16" x14ac:dyDescent="0.35">
@@ -18416,7 +18422,7 @@
         <v>2672</v>
       </c>
       <c r="P200" t="s">
-        <v>4355</v>
+        <v>4358</v>
       </c>
     </row>
     <row r="201" spans="7:16" x14ac:dyDescent="0.35">
@@ -18433,7 +18439,7 @@
         <v>3673</v>
       </c>
       <c r="P201" t="s">
-        <v>4356</v>
+        <v>4359</v>
       </c>
     </row>
     <row r="202" spans="7:16" x14ac:dyDescent="0.35">
@@ -18450,7 +18456,7 @@
         <v>3674</v>
       </c>
       <c r="P202" t="s">
-        <v>4357</v>
+        <v>4360</v>
       </c>
     </row>
     <row r="203" spans="7:16" x14ac:dyDescent="0.35">
@@ -18467,7 +18473,7 @@
         <v>3675</v>
       </c>
       <c r="P203" t="s">
-        <v>4358</v>
+        <v>4361</v>
       </c>
     </row>
     <row r="204" spans="7:16" x14ac:dyDescent="0.35">
@@ -18484,7 +18490,7 @@
         <v>3676</v>
       </c>
       <c r="P204" t="s">
-        <v>4359</v>
+        <v>4362</v>
       </c>
     </row>
     <row r="205" spans="7:16" x14ac:dyDescent="0.35">
@@ -18501,7 +18507,7 @@
         <v>960</v>
       </c>
       <c r="P205" t="s">
-        <v>4360</v>
+        <v>4363</v>
       </c>
     </row>
     <row r="206" spans="7:16" x14ac:dyDescent="0.35">
@@ -18518,7 +18524,7 @@
         <v>1025</v>
       </c>
       <c r="P206" t="s">
-        <v>4361</v>
+        <v>4364</v>
       </c>
     </row>
     <row r="207" spans="7:16" x14ac:dyDescent="0.35">
@@ -18535,7 +18541,7 @@
         <v>3677</v>
       </c>
       <c r="P207" t="s">
-        <v>4362</v>
+        <v>4365</v>
       </c>
     </row>
     <row r="208" spans="7:16" x14ac:dyDescent="0.35">
@@ -18552,7 +18558,7 @@
         <v>3678</v>
       </c>
       <c r="P208" t="s">
-        <v>4363</v>
+        <v>4366</v>
       </c>
     </row>
     <row r="209" spans="7:16" x14ac:dyDescent="0.35">
@@ -18569,7 +18575,7 @@
         <v>2382</v>
       </c>
       <c r="P209" t="s">
-        <v>4364</v>
+        <v>4367</v>
       </c>
     </row>
     <row r="210" spans="7:16" x14ac:dyDescent="0.35">
@@ -18586,7 +18592,7 @@
         <v>3679</v>
       </c>
       <c r="P210" t="s">
-        <v>4365</v>
+        <v>4368</v>
       </c>
     </row>
     <row r="211" spans="7:16" x14ac:dyDescent="0.35">
@@ -18603,7 +18609,7 @@
         <v>3680</v>
       </c>
       <c r="P211" t="s">
-        <v>4366</v>
+        <v>4369</v>
       </c>
     </row>
     <row r="212" spans="7:16" x14ac:dyDescent="0.35">
@@ -18620,7 +18626,7 @@
         <v>3681</v>
       </c>
       <c r="P212" t="s">
-        <v>4367</v>
+        <v>4370</v>
       </c>
     </row>
     <row r="213" spans="7:16" x14ac:dyDescent="0.35">
@@ -18637,7 +18643,7 @@
         <v>3682</v>
       </c>
       <c r="P213" t="s">
-        <v>4368</v>
+        <v>4371</v>
       </c>
     </row>
     <row r="214" spans="7:16" x14ac:dyDescent="0.35">
@@ -18654,7 +18660,7 @@
         <v>3683</v>
       </c>
       <c r="P214" t="s">
-        <v>4369</v>
+        <v>4372</v>
       </c>
     </row>
     <row r="215" spans="7:16" x14ac:dyDescent="0.35">
@@ -18671,7 +18677,7 @@
         <v>2758</v>
       </c>
       <c r="P215" t="s">
-        <v>4370</v>
+        <v>4373</v>
       </c>
     </row>
     <row r="216" spans="7:16" x14ac:dyDescent="0.35">
@@ -18688,7 +18694,7 @@
         <v>3185</v>
       </c>
       <c r="P216" t="s">
-        <v>4371</v>
+        <v>4374</v>
       </c>
     </row>
     <row r="217" spans="7:16" x14ac:dyDescent="0.35">
@@ -18705,7 +18711,7 @@
         <v>3684</v>
       </c>
       <c r="P217" t="s">
-        <v>4372</v>
+        <v>4375</v>
       </c>
     </row>
     <row r="218" spans="7:16" x14ac:dyDescent="0.35">
@@ -18722,7 +18728,7 @@
         <v>1181</v>
       </c>
       <c r="P218" t="s">
-        <v>4373</v>
+        <v>4376</v>
       </c>
     </row>
     <row r="219" spans="7:16" x14ac:dyDescent="0.35">
@@ -18739,7 +18745,7 @@
         <v>3685</v>
       </c>
       <c r="P219" t="s">
-        <v>4374</v>
+        <v>4377</v>
       </c>
     </row>
     <row r="220" spans="7:16" x14ac:dyDescent="0.35">
@@ -18756,7 +18762,7 @@
         <v>3686</v>
       </c>
       <c r="P220" t="s">
-        <v>4375</v>
+        <v>4378</v>
       </c>
     </row>
     <row r="221" spans="7:16" x14ac:dyDescent="0.35">
@@ -18773,7 +18779,7 @@
         <v>3687</v>
       </c>
       <c r="P221" t="s">
-        <v>4376</v>
+        <v>4379</v>
       </c>
     </row>
     <row r="222" spans="7:16" x14ac:dyDescent="0.35">
@@ -18790,7 +18796,7 @@
         <v>1692</v>
       </c>
       <c r="P222" t="s">
-        <v>4377</v>
+        <v>4380</v>
       </c>
     </row>
     <row r="223" spans="7:16" x14ac:dyDescent="0.35">
@@ -18807,7 +18813,7 @@
         <v>1093</v>
       </c>
       <c r="P223" t="s">
-        <v>4378</v>
+        <v>4381</v>
       </c>
     </row>
     <row r="224" spans="7:16" x14ac:dyDescent="0.35">
@@ -18824,7 +18830,7 @@
         <v>1099</v>
       </c>
       <c r="P224" t="s">
-        <v>4379</v>
+        <v>4382</v>
       </c>
     </row>
     <row r="225" spans="7:16" x14ac:dyDescent="0.35">
@@ -18841,7 +18847,7 @@
         <v>2117</v>
       </c>
       <c r="P225" t="s">
-        <v>4380</v>
+        <v>4383</v>
       </c>
     </row>
     <row r="226" spans="7:16" x14ac:dyDescent="0.35">
@@ -18858,7 +18864,7 @@
         <v>3688</v>
       </c>
       <c r="P226" t="s">
-        <v>4381</v>
+        <v>4384</v>
       </c>
     </row>
     <row r="227" spans="7:16" x14ac:dyDescent="0.35">
@@ -18875,7 +18881,7 @@
         <v>2580</v>
       </c>
       <c r="P227" t="s">
-        <v>4382</v>
+        <v>4385</v>
       </c>
     </row>
     <row r="228" spans="7:16" x14ac:dyDescent="0.35">
@@ -18892,7 +18898,7 @@
         <v>2574</v>
       </c>
       <c r="P228" t="s">
-        <v>4383</v>
+        <v>4386</v>
       </c>
     </row>
     <row r="229" spans="7:16" x14ac:dyDescent="0.35">
@@ -18909,7 +18915,7 @@
         <v>1514</v>
       </c>
       <c r="P229" t="s">
-        <v>4384</v>
+        <v>4387</v>
       </c>
     </row>
     <row r="230" spans="7:16" x14ac:dyDescent="0.35">
@@ -18926,7 +18932,7 @@
         <v>1079</v>
       </c>
       <c r="P230" t="s">
-        <v>4385</v>
+        <v>4388</v>
       </c>
     </row>
     <row r="231" spans="7:16" x14ac:dyDescent="0.35">
@@ -18943,7 +18949,7 @@
         <v>3689</v>
       </c>
       <c r="P231" t="s">
-        <v>4386</v>
+        <v>4389</v>
       </c>
     </row>
     <row r="232" spans="7:16" x14ac:dyDescent="0.35">
@@ -18960,7 +18966,7 @@
         <v>1750</v>
       </c>
       <c r="P232" t="s">
-        <v>4387</v>
+        <v>4390</v>
       </c>
     </row>
     <row r="233" spans="7:16" x14ac:dyDescent="0.35">
@@ -18977,7 +18983,7 @@
         <v>3690</v>
       </c>
       <c r="P233" t="s">
-        <v>4388</v>
+        <v>4391</v>
       </c>
     </row>
     <row r="234" spans="7:16" x14ac:dyDescent="0.35">
@@ -18994,7 +19000,7 @@
         <v>3691</v>
       </c>
       <c r="P234" t="s">
-        <v>4389</v>
+        <v>4392</v>
       </c>
     </row>
     <row r="235" spans="7:16" x14ac:dyDescent="0.35">
@@ -19011,7 +19017,7 @@
         <v>3692</v>
       </c>
       <c r="P235" t="s">
-        <v>4390</v>
+        <v>4393</v>
       </c>
     </row>
     <row r="236" spans="7:16" x14ac:dyDescent="0.35">
@@ -19028,7 +19034,7 @@
         <v>3693</v>
       </c>
       <c r="P236" t="s">
-        <v>4391</v>
+        <v>4394</v>
       </c>
     </row>
     <row r="237" spans="7:16" x14ac:dyDescent="0.35">
@@ -19045,7 +19051,7 @@
         <v>3694</v>
       </c>
       <c r="P237" t="s">
-        <v>4392</v>
+        <v>4395</v>
       </c>
     </row>
     <row r="238" spans="7:16" x14ac:dyDescent="0.35">
@@ -19062,7 +19068,7 @@
         <v>3695</v>
       </c>
       <c r="P238" t="s">
-        <v>4393</v>
+        <v>4396</v>
       </c>
     </row>
     <row r="239" spans="7:16" x14ac:dyDescent="0.35">
@@ -19079,7 +19085,7 @@
         <v>1077</v>
       </c>
       <c r="P239" t="s">
-        <v>4394</v>
+        <v>4397</v>
       </c>
     </row>
     <row r="240" spans="7:16" x14ac:dyDescent="0.35">
@@ -19096,7 +19102,7 @@
         <v>1879</v>
       </c>
       <c r="P240" t="s">
-        <v>4395</v>
+        <v>4398</v>
       </c>
     </row>
     <row r="241" spans="7:16" x14ac:dyDescent="0.35">
@@ -19113,7 +19119,7 @@
         <v>61</v>
       </c>
       <c r="P241" t="s">
-        <v>4396</v>
+        <v>4399</v>
       </c>
     </row>
     <row r="242" spans="7:16" x14ac:dyDescent="0.35">
@@ -19130,7 +19136,7 @@
         <v>3696</v>
       </c>
       <c r="P242" t="s">
-        <v>4397</v>
+        <v>4400</v>
       </c>
     </row>
     <row r="243" spans="7:16" x14ac:dyDescent="0.35">
@@ -19147,7 +19153,7 @@
         <v>3697</v>
       </c>
       <c r="P243" t="s">
-        <v>4398</v>
+        <v>4401</v>
       </c>
     </row>
     <row r="244" spans="7:16" x14ac:dyDescent="0.35">
@@ -19164,7 +19170,7 @@
         <v>3698</v>
       </c>
       <c r="P244" t="s">
-        <v>4399</v>
+        <v>4402</v>
       </c>
     </row>
     <row r="245" spans="7:16" x14ac:dyDescent="0.35">
@@ -19181,7 +19187,7 @@
         <v>2018</v>
       </c>
       <c r="P245" t="s">
-        <v>4400</v>
+        <v>4403</v>
       </c>
     </row>
     <row r="246" spans="7:16" x14ac:dyDescent="0.35">
@@ -19198,7 +19204,7 @@
         <v>3699</v>
       </c>
       <c r="P246" t="s">
-        <v>4401</v>
+        <v>4404</v>
       </c>
     </row>
     <row r="247" spans="7:16" x14ac:dyDescent="0.35">
@@ -19215,7 +19221,7 @@
         <v>3700</v>
       </c>
       <c r="P247" t="s">
-        <v>4402</v>
+        <v>4405</v>
       </c>
     </row>
     <row r="248" spans="7:16" x14ac:dyDescent="0.35">
@@ -19232,7 +19238,7 @@
         <v>2632</v>
       </c>
       <c r="P248" t="s">
-        <v>4403</v>
+        <v>4406</v>
       </c>
     </row>
     <row r="249" spans="7:16" x14ac:dyDescent="0.35">
@@ -19249,7 +19255,7 @@
         <v>3701</v>
       </c>
       <c r="P249" t="s">
-        <v>4404</v>
+        <v>4407</v>
       </c>
     </row>
     <row r="250" spans="7:16" x14ac:dyDescent="0.35">
@@ -19266,7 +19272,7 @@
         <v>3702</v>
       </c>
       <c r="P250" t="s">
-        <v>4405</v>
+        <v>4408</v>
       </c>
     </row>
     <row r="251" spans="7:16" x14ac:dyDescent="0.35">
@@ -19283,7 +19289,7 @@
         <v>1918</v>
       </c>
       <c r="P251" t="s">
-        <v>4406</v>
+        <v>4409</v>
       </c>
     </row>
     <row r="252" spans="7:16" x14ac:dyDescent="0.35">
@@ -19300,7 +19306,7 @@
         <v>3703</v>
       </c>
       <c r="P252" t="s">
-        <v>4407</v>
+        <v>4410</v>
       </c>
     </row>
     <row r="253" spans="7:16" x14ac:dyDescent="0.35">
@@ -19317,7 +19323,7 @@
         <v>1342</v>
       </c>
       <c r="P253" t="s">
-        <v>4408</v>
+        <v>4411</v>
       </c>
     </row>
     <row r="254" spans="7:16" x14ac:dyDescent="0.35">
@@ -19334,7 +19340,7 @@
         <v>1803</v>
       </c>
       <c r="P254" t="s">
-        <v>4409</v>
+        <v>4412</v>
       </c>
     </row>
     <row r="255" spans="7:16" x14ac:dyDescent="0.35">
@@ -19351,7 +19357,7 @@
         <v>1021</v>
       </c>
       <c r="P255" t="s">
-        <v>4410</v>
+        <v>4413</v>
       </c>
     </row>
     <row r="256" spans="7:16" x14ac:dyDescent="0.35">
@@ -19368,7 +19374,7 @@
         <v>3704</v>
       </c>
       <c r="P256" t="s">
-        <v>4411</v>
+        <v>4414</v>
       </c>
     </row>
     <row r="257" spans="7:16" x14ac:dyDescent="0.35">
@@ -19385,7 +19391,7 @@
         <v>3705</v>
       </c>
       <c r="P257" t="s">
-        <v>4412</v>
+        <v>4415</v>
       </c>
     </row>
     <row r="258" spans="7:16" x14ac:dyDescent="0.35">
@@ -19402,7 +19408,7 @@
         <v>312</v>
       </c>
       <c r="P258" t="s">
-        <v>4413</v>
+        <v>4416</v>
       </c>
     </row>
     <row r="259" spans="7:16" x14ac:dyDescent="0.35">
@@ -19419,7 +19425,7 @@
         <v>2158</v>
       </c>
       <c r="P259" t="s">
-        <v>4414</v>
+        <v>4417</v>
       </c>
     </row>
     <row r="260" spans="7:16" x14ac:dyDescent="0.35">
@@ -19436,7 +19442,7 @@
         <v>3706</v>
       </c>
       <c r="P260" t="s">
-        <v>4415</v>
+        <v>4418</v>
       </c>
     </row>
     <row r="261" spans="7:16" x14ac:dyDescent="0.35">
@@ -19453,7 +19459,7 @@
         <v>3707</v>
       </c>
       <c r="P261" t="s">
-        <v>4416</v>
+        <v>4419</v>
       </c>
     </row>
     <row r="262" spans="7:16" x14ac:dyDescent="0.35">
@@ -19470,7 +19476,7 @@
         <v>1795</v>
       </c>
       <c r="P262" t="s">
-        <v>4417</v>
+        <v>4420</v>
       </c>
     </row>
     <row r="263" spans="7:16" x14ac:dyDescent="0.35">
@@ -19487,7 +19493,7 @@
         <v>2757</v>
       </c>
       <c r="P263" t="s">
-        <v>4418</v>
+        <v>4421</v>
       </c>
     </row>
     <row r="264" spans="7:16" x14ac:dyDescent="0.35">
@@ -19504,7 +19510,7 @@
         <v>3708</v>
       </c>
       <c r="P264" t="s">
-        <v>4419</v>
+        <v>4422</v>
       </c>
     </row>
     <row r="265" spans="7:16" x14ac:dyDescent="0.35">
@@ -19521,7 +19527,7 @@
         <v>2045</v>
       </c>
       <c r="P265" t="s">
-        <v>4420</v>
+        <v>4423</v>
       </c>
     </row>
     <row r="266" spans="7:16" x14ac:dyDescent="0.35">
@@ -19538,7 +19544,7 @@
         <v>1876</v>
       </c>
       <c r="P266" t="s">
-        <v>4421</v>
+        <v>4424</v>
       </c>
     </row>
     <row r="267" spans="7:16" x14ac:dyDescent="0.35">
@@ -19555,7 +19561,7 @@
         <v>3709</v>
       </c>
       <c r="P267" t="s">
-        <v>4422</v>
+        <v>4425</v>
       </c>
     </row>
     <row r="268" spans="7:16" x14ac:dyDescent="0.35">
@@ -19572,7 +19578,7 @@
         <v>3710</v>
       </c>
       <c r="P268" t="s">
-        <v>4423</v>
+        <v>4426</v>
       </c>
     </row>
     <row r="269" spans="7:16" x14ac:dyDescent="0.35">
@@ -19589,7 +19595,7 @@
         <v>1804</v>
       </c>
       <c r="P269" t="s">
-        <v>4424</v>
+        <v>4427</v>
       </c>
     </row>
     <row r="270" spans="7:16" x14ac:dyDescent="0.35">
@@ -19606,7 +19612,7 @@
         <v>3711</v>
       </c>
       <c r="P270" t="s">
-        <v>4425</v>
+        <v>4428</v>
       </c>
     </row>
     <row r="271" spans="7:16" x14ac:dyDescent="0.35">
@@ -19623,7 +19629,7 @@
         <v>3712</v>
       </c>
       <c r="P271" t="s">
-        <v>4426</v>
+        <v>4429</v>
       </c>
     </row>
     <row r="272" spans="7:16" x14ac:dyDescent="0.35">
@@ -19640,7 +19646,7 @@
         <v>3713</v>
       </c>
       <c r="P272" t="s">
-        <v>4427</v>
+        <v>4430</v>
       </c>
     </row>
     <row r="273" spans="7:16" x14ac:dyDescent="0.35">
@@ -19657,7 +19663,7 @@
         <v>3714</v>
       </c>
       <c r="P273" t="s">
-        <v>4428</v>
+        <v>4431</v>
       </c>
     </row>
     <row r="274" spans="7:16" x14ac:dyDescent="0.35">
@@ -19674,7 +19680,7 @@
         <v>3715</v>
       </c>
       <c r="P274" t="s">
-        <v>4429</v>
+        <v>4432</v>
       </c>
     </row>
     <row r="275" spans="7:16" x14ac:dyDescent="0.35">
@@ -19691,7 +19697,7 @@
         <v>3716</v>
       </c>
       <c r="P275" t="s">
-        <v>4430</v>
+        <v>4433</v>
       </c>
     </row>
     <row r="276" spans="7:16" x14ac:dyDescent="0.35">
@@ -19708,7 +19714,7 @@
         <v>3717</v>
       </c>
       <c r="P276" t="s">
-        <v>4431</v>
+        <v>4434</v>
       </c>
     </row>
     <row r="277" spans="7:16" x14ac:dyDescent="0.35">
@@ -19725,7 +19731,7 @@
         <v>3718</v>
       </c>
       <c r="P277" t="s">
-        <v>4432</v>
+        <v>4435</v>
       </c>
     </row>
     <row r="278" spans="7:16" x14ac:dyDescent="0.35">
@@ -19742,7 +19748,7 @@
         <v>3719</v>
       </c>
       <c r="P278" t="s">
-        <v>4433</v>
+        <v>4436</v>
       </c>
     </row>
     <row r="279" spans="7:16" x14ac:dyDescent="0.35">
@@ -19759,7 +19765,7 @@
         <v>3720</v>
       </c>
       <c r="P279" t="s">
-        <v>4434</v>
+        <v>4437</v>
       </c>
     </row>
     <row r="280" spans="7:16" x14ac:dyDescent="0.35">
@@ -19776,7 +19782,7 @@
         <v>2061</v>
       </c>
       <c r="P280" t="s">
-        <v>4435</v>
+        <v>4438</v>
       </c>
     </row>
     <row r="281" spans="7:16" x14ac:dyDescent="0.35">
@@ -19793,7 +19799,7 @@
         <v>3721</v>
       </c>
       <c r="P281" t="s">
-        <v>4436</v>
+        <v>4439</v>
       </c>
     </row>
     <row r="282" spans="7:16" x14ac:dyDescent="0.35">
@@ -19810,7 +19816,7 @@
         <v>1153</v>
       </c>
       <c r="P282" t="s">
-        <v>4437</v>
+        <v>4440</v>
       </c>
     </row>
     <row r="283" spans="7:16" x14ac:dyDescent="0.35">
@@ -19827,7 +19833,7 @@
         <v>3722</v>
       </c>
       <c r="P283" t="s">
-        <v>4438</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="284" spans="7:16" x14ac:dyDescent="0.35">
@@ -19844,7 +19850,7 @@
         <v>3723</v>
       </c>
       <c r="P284" t="s">
-        <v>4439</v>
+        <v>4442</v>
       </c>
     </row>
     <row r="285" spans="7:16" x14ac:dyDescent="0.35">
@@ -19861,7 +19867,7 @@
         <v>2941</v>
       </c>
       <c r="P285" t="s">
-        <v>4440</v>
+        <v>4443</v>
       </c>
     </row>
     <row r="286" spans="7:16" x14ac:dyDescent="0.35">
@@ -19878,7 +19884,7 @@
         <v>3724</v>
       </c>
       <c r="P286" t="s">
-        <v>4441</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="287" spans="7:16" x14ac:dyDescent="0.35">
@@ -19895,7 +19901,7 @@
         <v>1630</v>
       </c>
       <c r="P287" t="s">
-        <v>4442</v>
+        <v>4445</v>
       </c>
     </row>
     <row r="288" spans="7:16" x14ac:dyDescent="0.35">
@@ -19912,7 +19918,7 @@
         <v>624</v>
       </c>
       <c r="P288" t="s">
-        <v>4443</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="289" spans="7:16" x14ac:dyDescent="0.35">
@@ -19929,7 +19935,7 @@
         <v>2512</v>
       </c>
       <c r="P289" t="s">
-        <v>4444</v>
+        <v>4447</v>
       </c>
     </row>
     <row r="290" spans="7:16" x14ac:dyDescent="0.35">
@@ -19946,7 +19952,7 @@
         <v>794</v>
       </c>
       <c r="P290" t="s">
-        <v>4445</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="291" spans="7:16" x14ac:dyDescent="0.35">
@@ -19963,7 +19969,7 @@
         <v>995</v>
       </c>
       <c r="P291" t="s">
-        <v>4446</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="292" spans="7:16" x14ac:dyDescent="0.35">
@@ -19980,7 +19986,7 @@
         <v>3725</v>
       </c>
       <c r="P292" t="s">
-        <v>4447</v>
+        <v>4450</v>
       </c>
     </row>
     <row r="293" spans="7:16" x14ac:dyDescent="0.35">
@@ -19997,7 +20003,7 @@
         <v>1177</v>
       </c>
       <c r="P293" t="s">
-        <v>4448</v>
+        <v>4451</v>
       </c>
     </row>
     <row r="294" spans="7:16" x14ac:dyDescent="0.35">
@@ -20014,7 +20020,7 @@
         <v>2800</v>
       </c>
       <c r="P294" t="s">
-        <v>4449</v>
+        <v>4452</v>
       </c>
     </row>
     <row r="295" spans="7:16" x14ac:dyDescent="0.35">
@@ -20031,7 +20037,7 @@
         <v>3726</v>
       </c>
       <c r="P295" t="s">
-        <v>4450</v>
+        <v>4453</v>
       </c>
     </row>
     <row r="296" spans="7:16" x14ac:dyDescent="0.35">
@@ -20048,7 +20054,7 @@
         <v>1262</v>
       </c>
       <c r="P296" t="s">
-        <v>4451</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="297" spans="7:16" x14ac:dyDescent="0.35">
@@ -20065,7 +20071,7 @@
         <v>3727</v>
       </c>
       <c r="P297" t="s">
-        <v>4452</v>
+        <v>4455</v>
       </c>
     </row>
     <row r="298" spans="7:16" x14ac:dyDescent="0.35">
@@ -20082,7 +20088,7 @@
         <v>3728</v>
       </c>
       <c r="P298" t="s">
-        <v>4453</v>
+        <v>4456</v>
       </c>
     </row>
     <row r="299" spans="7:16" x14ac:dyDescent="0.35">
@@ -20099,7 +20105,7 @@
         <v>2528</v>
       </c>
       <c r="P299" t="s">
-        <v>4454</v>
+        <v>4457</v>
       </c>
     </row>
     <row r="300" spans="7:16" x14ac:dyDescent="0.35">
@@ -20116,7 +20122,7 @@
         <v>3729</v>
       </c>
       <c r="P300" t="s">
-        <v>4455</v>
+        <v>4458</v>
       </c>
     </row>
     <row r="301" spans="7:16" x14ac:dyDescent="0.35">
@@ -20133,7 +20139,7 @@
         <v>3730</v>
       </c>
       <c r="P301" t="s">
-        <v>4456</v>
+        <v>4459</v>
       </c>
     </row>
     <row r="302" spans="7:16" x14ac:dyDescent="0.35">
@@ -20150,7 +20156,7 @@
         <v>3731</v>
       </c>
       <c r="P302" t="s">
-        <v>4457</v>
+        <v>4460</v>
       </c>
     </row>
     <row r="303" spans="7:16" x14ac:dyDescent="0.35">
@@ -20167,7 +20173,7 @@
         <v>2682</v>
       </c>
       <c r="P303" t="s">
-        <v>4458</v>
+        <v>4461</v>
       </c>
     </row>
     <row r="304" spans="7:16" x14ac:dyDescent="0.35">
@@ -20184,7 +20190,7 @@
         <v>3732</v>
       </c>
       <c r="P304" t="s">
-        <v>4459</v>
+        <v>4462</v>
       </c>
     </row>
     <row r="305" spans="7:16" x14ac:dyDescent="0.35">
@@ -20201,7 +20207,7 @@
         <v>2799</v>
       </c>
       <c r="P305" t="s">
-        <v>4460</v>
+        <v>4463</v>
       </c>
     </row>
     <row r="306" spans="7:16" x14ac:dyDescent="0.35">
@@ -20218,7 +20224,7 @@
         <v>150</v>
       </c>
       <c r="P306" t="s">
-        <v>4461</v>
+        <v>4464</v>
       </c>
     </row>
     <row r="307" spans="7:16" x14ac:dyDescent="0.35">
@@ -20235,7 +20241,7 @@
         <v>3733</v>
       </c>
       <c r="P307" t="s">
-        <v>4462</v>
+        <v>4465</v>
       </c>
     </row>
     <row r="308" spans="7:16" x14ac:dyDescent="0.35">
@@ -20252,7 +20258,7 @@
         <v>1044</v>
       </c>
       <c r="P308" t="s">
-        <v>4463</v>
+        <v>4466</v>
       </c>
     </row>
     <row r="309" spans="7:16" x14ac:dyDescent="0.35">
@@ -20269,7 +20275,7 @@
         <v>1664</v>
       </c>
       <c r="P309" t="s">
-        <v>4464</v>
+        <v>4467</v>
       </c>
     </row>
     <row r="310" spans="7:16" x14ac:dyDescent="0.35">
@@ -20286,7 +20292,7 @@
         <v>1783</v>
       </c>
       <c r="P310" t="s">
-        <v>4465</v>
+        <v>4468</v>
       </c>
     </row>
     <row r="311" spans="7:16" x14ac:dyDescent="0.35">
@@ -20303,7 +20309,7 @@
         <v>3734</v>
       </c>
       <c r="P311" t="s">
-        <v>4466</v>
+        <v>4469</v>
       </c>
     </row>
     <row r="312" spans="7:16" x14ac:dyDescent="0.35">
@@ -20320,7 +20326,7 @@
         <v>3735</v>
       </c>
       <c r="P312" t="s">
-        <v>4467</v>
+        <v>4470</v>
       </c>
     </row>
     <row r="313" spans="7:16" x14ac:dyDescent="0.35">
@@ -20337,7 +20343,7 @@
         <v>1447</v>
       </c>
       <c r="P313" t="s">
-        <v>4468</v>
+        <v>4471</v>
       </c>
     </row>
     <row r="314" spans="7:16" x14ac:dyDescent="0.35">
@@ -20354,7 +20360,7 @@
         <v>3736</v>
       </c>
       <c r="P314" t="s">
-        <v>4469</v>
+        <v>4472</v>
       </c>
     </row>
     <row r="315" spans="7:16" x14ac:dyDescent="0.35">
@@ -20371,7 +20377,7 @@
         <v>1140</v>
       </c>
       <c r="P315" t="s">
-        <v>4470</v>
+        <v>4473</v>
       </c>
     </row>
     <row r="316" spans="7:16" x14ac:dyDescent="0.35">
@@ -20388,7 +20394,7 @@
         <v>3737</v>
       </c>
       <c r="P316" t="s">
-        <v>4471</v>
+        <v>4474</v>
       </c>
     </row>
     <row r="317" spans="7:16" x14ac:dyDescent="0.35">
@@ -20405,7 +20411,7 @@
         <v>3738</v>
       </c>
       <c r="P317" t="s">
-        <v>4472</v>
+        <v>4475</v>
       </c>
     </row>
     <row r="318" spans="7:16" x14ac:dyDescent="0.35">
@@ -20422,7 +20428,7 @@
         <v>3739</v>
       </c>
       <c r="P318" t="s">
-        <v>4473</v>
+        <v>4476</v>
       </c>
     </row>
     <row r="319" spans="7:16" x14ac:dyDescent="0.35">
@@ -20439,7 +20445,7 @@
         <v>3740</v>
       </c>
       <c r="P319" t="s">
-        <v>4474</v>
+        <v>4477</v>
       </c>
     </row>
     <row r="320" spans="7:16" x14ac:dyDescent="0.35">
@@ -20456,7 +20462,7 @@
         <v>1767</v>
       </c>
       <c r="P320" t="s">
-        <v>4475</v>
+        <v>4478</v>
       </c>
     </row>
     <row r="321" spans="7:16" x14ac:dyDescent="0.35">
@@ -20473,7 +20479,7 @@
         <v>1640</v>
       </c>
       <c r="P321" t="s">
-        <v>4476</v>
+        <v>4479</v>
       </c>
     </row>
     <row r="322" spans="7:16" x14ac:dyDescent="0.35">
@@ -20490,7 +20496,7 @@
         <v>3741</v>
       </c>
       <c r="P322" t="s">
-        <v>4477</v>
+        <v>4480</v>
       </c>
     </row>
     <row r="323" spans="7:16" x14ac:dyDescent="0.35">
@@ -20507,7 +20513,7 @@
         <v>3742</v>
       </c>
       <c r="P323" t="s">
-        <v>4478</v>
+        <v>4481</v>
       </c>
     </row>
     <row r="324" spans="7:16" x14ac:dyDescent="0.35">
@@ -20524,7 +20530,7 @@
         <v>1384</v>
       </c>
       <c r="P324" t="s">
-        <v>4479</v>
+        <v>4482</v>
       </c>
     </row>
     <row r="325" spans="7:16" x14ac:dyDescent="0.35">
@@ -20541,7 +20547,7 @@
         <v>3743</v>
       </c>
       <c r="P325" t="s">
-        <v>4480</v>
+        <v>4483</v>
       </c>
     </row>
     <row r="326" spans="7:16" x14ac:dyDescent="0.35">
@@ -20558,7 +20564,7 @@
         <v>1199</v>
       </c>
       <c r="P326" t="s">
-        <v>4481</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="327" spans="7:16" x14ac:dyDescent="0.35">
@@ -20575,7 +20581,7 @@
         <v>3744</v>
       </c>
       <c r="P327" t="s">
-        <v>4482</v>
+        <v>4485</v>
       </c>
     </row>
     <row r="328" spans="7:16" x14ac:dyDescent="0.35">
@@ -20592,7 +20598,7 @@
         <v>662</v>
       </c>
       <c r="P328" t="s">
-        <v>4483</v>
+        <v>4486</v>
       </c>
     </row>
     <row r="329" spans="7:16" x14ac:dyDescent="0.35">
@@ -20609,7 +20615,7 @@
         <v>3745</v>
       </c>
       <c r="P329" t="s">
-        <v>4484</v>
+        <v>4487</v>
       </c>
     </row>
     <row r="330" spans="7:16" x14ac:dyDescent="0.35">
@@ -20626,7 +20632,7 @@
         <v>2112</v>
       </c>
       <c r="P330" t="s">
-        <v>4485</v>
+        <v>4488</v>
       </c>
     </row>
     <row r="331" spans="7:16" x14ac:dyDescent="0.35">
@@ -20643,7 +20649,7 @@
         <v>322</v>
       </c>
       <c r="P331" t="s">
-        <v>4486</v>
+        <v>4489</v>
       </c>
     </row>
     <row r="332" spans="7:16" x14ac:dyDescent="0.35">
@@ -20660,7 +20666,7 @@
         <v>3746</v>
       </c>
       <c r="P332" t="s">
-        <v>4487</v>
+        <v>4490</v>
       </c>
     </row>
     <row r="333" spans="7:16" x14ac:dyDescent="0.35">
@@ -20677,7 +20683,7 @@
         <v>3747</v>
       </c>
       <c r="P333" t="s">
-        <v>4488</v>
+        <v>4491</v>
       </c>
     </row>
     <row r="334" spans="7:16" x14ac:dyDescent="0.35">
@@ -20694,7 +20700,7 @@
         <v>3748</v>
       </c>
       <c r="P334" t="s">
-        <v>4489</v>
+        <v>4492</v>
       </c>
     </row>
     <row r="335" spans="7:16" x14ac:dyDescent="0.35">
@@ -20711,7 +20717,7 @@
         <v>3749</v>
       </c>
       <c r="P335" t="s">
-        <v>4490</v>
+        <v>4493</v>
       </c>
     </row>
     <row r="336" spans="7:16" x14ac:dyDescent="0.35">
@@ -20728,7 +20734,7 @@
         <v>3750</v>
       </c>
       <c r="P336" t="s">
-        <v>4491</v>
+        <v>4494</v>
       </c>
     </row>
     <row r="337" spans="7:16" x14ac:dyDescent="0.35">
@@ -20745,7 +20751,7 @@
         <v>3751</v>
       </c>
       <c r="P337" t="s">
-        <v>4492</v>
+        <v>4495</v>
       </c>
     </row>
     <row r="338" spans="7:16" x14ac:dyDescent="0.35">
@@ -20762,7 +20768,7 @@
         <v>3752</v>
       </c>
       <c r="P338" t="s">
-        <v>4493</v>
+        <v>4496</v>
       </c>
     </row>
     <row r="339" spans="7:16" x14ac:dyDescent="0.35">
@@ -20776,7 +20782,7 @@
         <v>3753</v>
       </c>
       <c r="P339" t="s">
-        <v>4494</v>
+        <v>4497</v>
       </c>
     </row>
     <row r="340" spans="7:16" x14ac:dyDescent="0.35">
@@ -20790,7 +20796,7 @@
         <v>3754</v>
       </c>
       <c r="P340" t="s">
-        <v>4495</v>
+        <v>4498</v>
       </c>
     </row>
     <row r="341" spans="7:16" x14ac:dyDescent="0.35">
@@ -20804,7 +20810,7 @@
         <v>2131</v>
       </c>
       <c r="P341" t="s">
-        <v>4496</v>
+        <v>4499</v>
       </c>
     </row>
     <row r="342" spans="7:16" x14ac:dyDescent="0.35">
@@ -20818,7 +20824,7 @@
         <v>3755</v>
       </c>
       <c r="P342" t="s">
-        <v>4497</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="343" spans="7:16" x14ac:dyDescent="0.35">
@@ -20832,7 +20838,7 @@
         <v>1410</v>
       </c>
       <c r="P343" t="s">
-        <v>4498</v>
+        <v>4501</v>
       </c>
     </row>
     <row r="344" spans="7:16" x14ac:dyDescent="0.35">
@@ -20846,7 +20852,7 @@
         <v>3756</v>
       </c>
       <c r="P344" t="s">
-        <v>4499</v>
+        <v>4502</v>
       </c>
     </row>
     <row r="345" spans="7:16" x14ac:dyDescent="0.35">
@@ -20860,7 +20866,7 @@
         <v>3757</v>
       </c>
       <c r="P345" t="s">
-        <v>4500</v>
+        <v>4503</v>
       </c>
     </row>
     <row r="346" spans="7:16" x14ac:dyDescent="0.35">
@@ -20874,7 +20880,7 @@
         <v>3758</v>
       </c>
       <c r="P346" t="s">
-        <v>4501</v>
+        <v>4504</v>
       </c>
     </row>
     <row r="347" spans="7:16" x14ac:dyDescent="0.35">
@@ -20888,7 +20894,7 @@
         <v>3759</v>
       </c>
       <c r="P347" t="s">
-        <v>4502</v>
+        <v>4505</v>
       </c>
     </row>
     <row r="348" spans="7:16" x14ac:dyDescent="0.35">
@@ -20902,7 +20908,7 @@
         <v>1060</v>
       </c>
       <c r="P348" t="s">
-        <v>4503</v>
+        <v>4506</v>
       </c>
     </row>
     <row r="349" spans="7:16" x14ac:dyDescent="0.35">
@@ -20916,7 +20922,7 @@
         <v>1283</v>
       </c>
       <c r="P349" t="s">
-        <v>4504</v>
+        <v>4507</v>
       </c>
     </row>
     <row r="350" spans="7:16" x14ac:dyDescent="0.35">
@@ -20930,7 +20936,7 @@
         <v>1739</v>
       </c>
       <c r="P350" t="s">
-        <v>4505</v>
+        <v>4508</v>
       </c>
     </row>
     <row r="351" spans="7:16" x14ac:dyDescent="0.35">
@@ -20944,7 +20950,7 @@
         <v>3760</v>
       </c>
       <c r="P351" t="s">
-        <v>4506</v>
+        <v>4509</v>
       </c>
     </row>
     <row r="352" spans="7:16" x14ac:dyDescent="0.35">
@@ -20958,7 +20964,7 @@
         <v>880</v>
       </c>
       <c r="P352" t="s">
-        <v>4507</v>
+        <v>4510</v>
       </c>
     </row>
     <row r="353" spans="7:16" x14ac:dyDescent="0.35">
@@ -20972,7 +20978,7 @@
         <v>1916</v>
       </c>
       <c r="P353" t="s">
-        <v>4508</v>
+        <v>4511</v>
       </c>
     </row>
     <row r="354" spans="7:16" x14ac:dyDescent="0.35">
@@ -20986,7 +20992,7 @@
         <v>1842</v>
       </c>
       <c r="P354" t="s">
-        <v>4509</v>
+        <v>4512</v>
       </c>
     </row>
     <row r="355" spans="7:16" x14ac:dyDescent="0.35">
@@ -21000,7 +21006,7 @@
         <v>3761</v>
       </c>
       <c r="P355" t="s">
-        <v>4510</v>
+        <v>4513</v>
       </c>
     </row>
     <row r="356" spans="7:16" x14ac:dyDescent="0.35">
@@ -21014,7 +21020,7 @@
         <v>3762</v>
       </c>
       <c r="P356" t="s">
-        <v>4511</v>
+        <v>4514</v>
       </c>
     </row>
     <row r="357" spans="7:16" x14ac:dyDescent="0.35">
@@ -21028,7 +21034,7 @@
         <v>3763</v>
       </c>
       <c r="P357" t="s">
-        <v>4512</v>
+        <v>4515</v>
       </c>
     </row>
     <row r="358" spans="7:16" x14ac:dyDescent="0.35">
@@ -21042,7 +21048,7 @@
         <v>3764</v>
       </c>
       <c r="P358" t="s">
-        <v>4513</v>
+        <v>4516</v>
       </c>
     </row>
     <row r="359" spans="7:16" x14ac:dyDescent="0.35">
@@ -21056,7 +21062,7 @@
         <v>3765</v>
       </c>
       <c r="P359" t="s">
-        <v>4514</v>
+        <v>4517</v>
       </c>
     </row>
     <row r="360" spans="7:16" x14ac:dyDescent="0.35">
@@ -21070,7 +21076,7 @@
         <v>3766</v>
       </c>
       <c r="P360" t="s">
-        <v>4515</v>
+        <v>4518</v>
       </c>
     </row>
     <row r="361" spans="7:16" x14ac:dyDescent="0.35">
@@ -21084,7 +21090,7 @@
         <v>1544</v>
       </c>
       <c r="P361" t="s">
-        <v>4516</v>
+        <v>4519</v>
       </c>
     </row>
     <row r="362" spans="7:16" x14ac:dyDescent="0.35">
@@ -21098,7 +21104,7 @@
         <v>1390</v>
       </c>
       <c r="P362" t="s">
-        <v>4517</v>
+        <v>4520</v>
       </c>
     </row>
     <row r="363" spans="7:16" x14ac:dyDescent="0.35">
@@ -21112,7 +21118,7 @@
         <v>1871</v>
       </c>
       <c r="P363" t="s">
-        <v>4518</v>
+        <v>4521</v>
       </c>
     </row>
     <row r="364" spans="7:16" x14ac:dyDescent="0.35">
@@ -21126,7 +21132,7 @@
         <v>3767</v>
       </c>
       <c r="P364" t="s">
-        <v>4519</v>
+        <v>4522</v>
       </c>
     </row>
     <row r="365" spans="7:16" x14ac:dyDescent="0.35">
@@ -21140,7 +21146,7 @@
         <v>3768</v>
       </c>
       <c r="P365" t="s">
-        <v>4520</v>
+        <v>4523</v>
       </c>
     </row>
     <row r="366" spans="7:16" x14ac:dyDescent="0.35">
@@ -21154,7 +21160,7 @@
         <v>3769</v>
       </c>
       <c r="P366" t="s">
-        <v>4521</v>
+        <v>4524</v>
       </c>
     </row>
     <row r="367" spans="7:16" x14ac:dyDescent="0.35">
@@ -21168,7 +21174,7 @@
         <v>3246</v>
       </c>
       <c r="P367" t="s">
-        <v>4522</v>
+        <v>4525</v>
       </c>
     </row>
     <row r="368" spans="7:16" x14ac:dyDescent="0.35">
@@ -21182,7 +21188,7 @@
         <v>3770</v>
       </c>
       <c r="P368" t="s">
-        <v>4523</v>
+        <v>4526</v>
       </c>
     </row>
     <row r="369" spans="7:16" x14ac:dyDescent="0.35">
@@ -21196,7 +21202,7 @@
         <v>79</v>
       </c>
       <c r="P369" t="s">
-        <v>4524</v>
+        <v>4527</v>
       </c>
     </row>
     <row r="370" spans="7:16" x14ac:dyDescent="0.35">
@@ -21210,7 +21216,7 @@
         <v>1357</v>
       </c>
       <c r="P370" t="s">
-        <v>4525</v>
+        <v>4528</v>
       </c>
     </row>
     <row r="371" spans="7:16" x14ac:dyDescent="0.35">
@@ -21224,7 +21230,7 @@
         <v>3771</v>
       </c>
       <c r="P371" t="s">
-        <v>4526</v>
+        <v>4529</v>
       </c>
     </row>
     <row r="372" spans="7:16" x14ac:dyDescent="0.35">
@@ -21238,7 +21244,7 @@
         <v>3772</v>
       </c>
       <c r="P372" t="s">
-        <v>4527</v>
+        <v>4530</v>
       </c>
     </row>
     <row r="373" spans="7:16" x14ac:dyDescent="0.35">
@@ -21252,7 +21258,7 @@
         <v>2202</v>
       </c>
       <c r="P373" t="s">
-        <v>4528</v>
+        <v>4531</v>
       </c>
     </row>
     <row r="374" spans="7:16" x14ac:dyDescent="0.35">
@@ -21266,7 +21272,7 @@
         <v>2790</v>
       </c>
       <c r="P374" t="s">
-        <v>4529</v>
+        <v>4532</v>
       </c>
     </row>
     <row r="375" spans="7:16" x14ac:dyDescent="0.35">
@@ -21280,7 +21286,7 @@
         <v>1282</v>
       </c>
       <c r="P375" t="s">
-        <v>4530</v>
+        <v>4533</v>
       </c>
     </row>
     <row r="376" spans="7:16" x14ac:dyDescent="0.35">
@@ -21294,7 +21300,7 @@
         <v>3773</v>
       </c>
       <c r="P376" t="s">
-        <v>4531</v>
+        <v>4534</v>
       </c>
     </row>
     <row r="377" spans="7:16" x14ac:dyDescent="0.35">
@@ -21308,7 +21314,7 @@
         <v>3774</v>
       </c>
       <c r="P377" t="s">
-        <v>4532</v>
+        <v>4535</v>
       </c>
     </row>
     <row r="378" spans="7:16" x14ac:dyDescent="0.35">
@@ -21322,7 +21328,7 @@
         <v>3775</v>
       </c>
       <c r="P378" t="s">
-        <v>4533</v>
+        <v>4536</v>
       </c>
     </row>
     <row r="379" spans="7:16" x14ac:dyDescent="0.35">
@@ -21336,7 +21342,7 @@
         <v>3776</v>
       </c>
       <c r="P379" t="s">
-        <v>4534</v>
+        <v>4537</v>
       </c>
     </row>
     <row r="380" spans="7:16" x14ac:dyDescent="0.35">
@@ -21350,7 +21356,7 @@
         <v>1496</v>
       </c>
       <c r="P380" t="s">
-        <v>4535</v>
+        <v>4538</v>
       </c>
     </row>
     <row r="381" spans="7:16" x14ac:dyDescent="0.35">
@@ -21364,7 +21370,7 @@
         <v>3777</v>
       </c>
       <c r="P381" t="s">
-        <v>4536</v>
+        <v>4539</v>
       </c>
     </row>
     <row r="382" spans="7:16" x14ac:dyDescent="0.35">
@@ -21378,7 +21384,7 @@
         <v>2029</v>
       </c>
       <c r="P382" t="s">
-        <v>4537</v>
+        <v>4540</v>
       </c>
     </row>
     <row r="383" spans="7:16" x14ac:dyDescent="0.35">
@@ -21392,7 +21398,7 @@
         <v>3778</v>
       </c>
       <c r="P383" t="s">
-        <v>4538</v>
+        <v>4541</v>
       </c>
     </row>
     <row r="384" spans="7:16" x14ac:dyDescent="0.35">
@@ -21406,7 +21412,7 @@
         <v>3779</v>
       </c>
       <c r="P384" t="s">
-        <v>4539</v>
+        <v>4542</v>
       </c>
     </row>
     <row r="385" spans="7:16" x14ac:dyDescent="0.35">
@@ -21420,7 +21426,7 @@
         <v>3780</v>
       </c>
       <c r="P385" t="s">
-        <v>4540</v>
+        <v>4543</v>
       </c>
     </row>
     <row r="386" spans="7:16" x14ac:dyDescent="0.35">
@@ -21434,7 +21440,7 @@
         <v>3781</v>
       </c>
       <c r="P386" t="s">
-        <v>4541</v>
+        <v>4544</v>
       </c>
     </row>
     <row r="387" spans="7:16" x14ac:dyDescent="0.35">
@@ -21448,7 +21454,7 @@
         <v>1897</v>
       </c>
       <c r="P387" t="s">
-        <v>4542</v>
+        <v>4545</v>
       </c>
     </row>
     <row r="388" spans="7:16" x14ac:dyDescent="0.35">
@@ -21462,7 +21468,7 @@
         <v>1337</v>
       </c>
       <c r="P388" t="s">
-        <v>4543</v>
+        <v>4546</v>
       </c>
     </row>
     <row r="389" spans="7:16" x14ac:dyDescent="0.35">
@@ -21476,7 +21482,7 @@
         <v>3782</v>
       </c>
       <c r="P389" t="s">
-        <v>4544</v>
+        <v>4547</v>
       </c>
     </row>
     <row r="390" spans="7:16" x14ac:dyDescent="0.35">
@@ -21490,7 +21496,7 @@
         <v>3783</v>
       </c>
       <c r="P390" t="s">
-        <v>4545</v>
+        <v>4548</v>
       </c>
     </row>
     <row r="391" spans="7:16" x14ac:dyDescent="0.35">
@@ -21504,7 +21510,7 @@
         <v>3784</v>
       </c>
       <c r="P391" t="s">
-        <v>4546</v>
+        <v>4549</v>
       </c>
     </row>
     <row r="392" spans="7:16" x14ac:dyDescent="0.35">
@@ -21518,7 +21524,7 @@
         <v>3785</v>
       </c>
       <c r="P392" t="s">
-        <v>4547</v>
+        <v>4550</v>
       </c>
     </row>
     <row r="393" spans="7:16" x14ac:dyDescent="0.35">
@@ -21532,7 +21538,7 @@
         <v>3786</v>
       </c>
       <c r="P393" t="s">
-        <v>4548</v>
+        <v>4551</v>
       </c>
     </row>
     <row r="394" spans="7:16" x14ac:dyDescent="0.35">
@@ -21546,7 +21552,7 @@
         <v>957</v>
       </c>
       <c r="P394" t="s">
-        <v>4549</v>
+        <v>4552</v>
       </c>
     </row>
     <row r="395" spans="7:16" x14ac:dyDescent="0.35">
@@ -21560,7 +21566,7 @@
         <v>983</v>
       </c>
       <c r="P395" t="s">
-        <v>4550</v>
+        <v>4553</v>
       </c>
     </row>
     <row r="396" spans="7:16" x14ac:dyDescent="0.35">
@@ -21574,7 +21580,7 @@
         <v>1278</v>
       </c>
       <c r="P396" t="s">
-        <v>4551</v>
+        <v>4554</v>
       </c>
     </row>
     <row r="397" spans="7:16" x14ac:dyDescent="0.35">
@@ -21588,7 +21594,7 @@
         <v>3787</v>
       </c>
       <c r="P397" t="s">
-        <v>4552</v>
+        <v>4555</v>
       </c>
     </row>
     <row r="398" spans="7:16" x14ac:dyDescent="0.35">
@@ -21602,7 +21608,7 @@
         <v>1665</v>
       </c>
       <c r="P398" t="s">
-        <v>4553</v>
+        <v>4556</v>
       </c>
     </row>
     <row r="399" spans="7:16" x14ac:dyDescent="0.35">
@@ -21616,7 +21622,7 @@
         <v>199</v>
       </c>
       <c r="P399" t="s">
-        <v>4554</v>
+        <v>4557</v>
       </c>
     </row>
     <row r="400" spans="7:16" x14ac:dyDescent="0.35">
@@ -21630,7 +21636,7 @@
         <v>3788</v>
       </c>
       <c r="P400" t="s">
-        <v>4555</v>
+        <v>4558</v>
       </c>
     </row>
     <row r="401" spans="7:16" x14ac:dyDescent="0.35">
@@ -21644,7 +21650,7 @@
         <v>3789</v>
       </c>
       <c r="P401" t="s">
-        <v>4556</v>
+        <v>4559</v>
       </c>
     </row>
     <row r="402" spans="7:16" x14ac:dyDescent="0.35">
@@ -21658,7 +21664,7 @@
         <v>330</v>
       </c>
       <c r="P402" t="s">
-        <v>4557</v>
+        <v>4560</v>
       </c>
     </row>
     <row r="403" spans="7:16" x14ac:dyDescent="0.35">
@@ -21672,7 +21678,7 @@
         <v>2411</v>
       </c>
       <c r="P403" t="s">
-        <v>4558</v>
+        <v>4561</v>
       </c>
     </row>
     <row r="404" spans="7:16" x14ac:dyDescent="0.35">
@@ -21686,7 +21692,7 @@
         <v>1338</v>
       </c>
       <c r="P404" t="s">
-        <v>4559</v>
+        <v>4562</v>
       </c>
     </row>
     <row r="405" spans="7:16" x14ac:dyDescent="0.35">
@@ -21700,7 +21706,7 @@
         <v>2539</v>
       </c>
       <c r="P405" t="s">
-        <v>4560</v>
+        <v>4563</v>
       </c>
     </row>
     <row r="406" spans="7:16" x14ac:dyDescent="0.35">
@@ -21714,7 +21720,7 @@
         <v>1148</v>
       </c>
       <c r="P406" t="s">
-        <v>4561</v>
+        <v>4564</v>
       </c>
     </row>
     <row r="407" spans="7:16" x14ac:dyDescent="0.35">
@@ -21728,7 +21734,7 @@
         <v>383</v>
       </c>
       <c r="P407" t="s">
-        <v>4562</v>
+        <v>4565</v>
       </c>
     </row>
     <row r="408" spans="7:16" x14ac:dyDescent="0.35">
@@ -21742,7 +21748,7 @@
         <v>2609</v>
       </c>
       <c r="P408" t="s">
-        <v>4563</v>
+        <v>4566</v>
       </c>
     </row>
     <row r="409" spans="7:16" x14ac:dyDescent="0.35">
@@ -21756,7 +21762,7 @@
         <v>3790</v>
       </c>
       <c r="P409" t="s">
-        <v>4564</v>
+        <v>4567</v>
       </c>
     </row>
     <row r="410" spans="7:16" x14ac:dyDescent="0.35">
@@ -21770,7 +21776,7 @@
         <v>3791</v>
       </c>
       <c r="P410" t="s">
-        <v>4565</v>
+        <v>4568</v>
       </c>
     </row>
     <row r="411" spans="7:16" x14ac:dyDescent="0.35">
@@ -21784,7 +21790,7 @@
         <v>3792</v>
       </c>
       <c r="P411" t="s">
-        <v>4566</v>
+        <v>4569</v>
       </c>
     </row>
     <row r="412" spans="7:16" x14ac:dyDescent="0.35">
@@ -21798,7 +21804,7 @@
         <v>935</v>
       </c>
       <c r="P412" t="s">
-        <v>4567</v>
+        <v>4570</v>
       </c>
     </row>
     <row r="413" spans="7:16" x14ac:dyDescent="0.35">
@@ -21812,7 +21818,7 @@
         <v>2666</v>
       </c>
       <c r="P413" t="s">
-        <v>4568</v>
+        <v>4571</v>
       </c>
     </row>
     <row r="414" spans="7:16" x14ac:dyDescent="0.35">
@@ -21826,7 +21832,7 @@
         <v>3793</v>
       </c>
       <c r="P414" t="s">
-        <v>4569</v>
+        <v>4572</v>
       </c>
     </row>
     <row r="415" spans="7:16" x14ac:dyDescent="0.35">
@@ -21840,7 +21846,7 @@
         <v>1629</v>
       </c>
       <c r="P415" t="s">
-        <v>4570</v>
+        <v>4573</v>
       </c>
     </row>
     <row r="416" spans="7:16" x14ac:dyDescent="0.35">
@@ -21854,7 +21860,7 @@
         <v>2128</v>
       </c>
       <c r="P416" t="s">
-        <v>4571</v>
+        <v>4574</v>
       </c>
     </row>
     <row r="417" spans="7:16" x14ac:dyDescent="0.35">
@@ -21868,7 +21874,7 @@
         <v>1413</v>
       </c>
       <c r="P417" t="s">
-        <v>4572</v>
+        <v>4575</v>
       </c>
     </row>
     <row r="418" spans="7:16" x14ac:dyDescent="0.35">
@@ -21882,7 +21888,7 @@
         <v>3794</v>
       </c>
       <c r="P418" t="s">
-        <v>4573</v>
+        <v>4576</v>
       </c>
     </row>
     <row r="419" spans="7:16" x14ac:dyDescent="0.35">
@@ -21896,7 +21902,7 @@
         <v>2157</v>
       </c>
       <c r="P419" t="s">
-        <v>4574</v>
+        <v>4577</v>
       </c>
     </row>
     <row r="420" spans="7:16" x14ac:dyDescent="0.35">
@@ -21910,7 +21916,7 @@
         <v>3795</v>
       </c>
       <c r="P420" t="s">
-        <v>4575</v>
+        <v>4578</v>
       </c>
     </row>
     <row r="421" spans="7:16" x14ac:dyDescent="0.35">
@@ -21924,7 +21930,7 @@
         <v>3796</v>
       </c>
       <c r="P421" t="s">
-        <v>4576</v>
+        <v>4579</v>
       </c>
     </row>
     <row r="422" spans="7:16" x14ac:dyDescent="0.35">
@@ -21938,7 +21944,7 @@
         <v>3797</v>
       </c>
       <c r="P422" t="s">
-        <v>4577</v>
+        <v>4580</v>
       </c>
     </row>
     <row r="423" spans="7:16" x14ac:dyDescent="0.35">
@@ -21952,7 +21958,7 @@
         <v>3798</v>
       </c>
       <c r="P423" t="s">
-        <v>4578</v>
+        <v>4581</v>
       </c>
     </row>
     <row r="424" spans="7:16" x14ac:dyDescent="0.35">
@@ -21966,7 +21972,7 @@
         <v>3799</v>
       </c>
       <c r="P424" t="s">
-        <v>4579</v>
+        <v>4582</v>
       </c>
     </row>
     <row r="425" spans="7:16" x14ac:dyDescent="0.35">
@@ -21980,7 +21986,7 @@
         <v>929</v>
       </c>
       <c r="P425" t="s">
-        <v>4580</v>
+        <v>4583</v>
       </c>
     </row>
     <row r="426" spans="7:16" x14ac:dyDescent="0.35">
@@ -21994,7 +22000,7 @@
         <v>1087</v>
       </c>
       <c r="P426" t="s">
-        <v>4581</v>
+        <v>4584</v>
       </c>
     </row>
     <row r="427" spans="7:16" x14ac:dyDescent="0.35">
@@ -22008,7 +22014,7 @@
         <v>3800</v>
       </c>
       <c r="P427" t="s">
-        <v>4582</v>
+        <v>4585</v>
       </c>
     </row>
     <row r="428" spans="7:16" x14ac:dyDescent="0.35">
@@ -22022,7 +22028,7 @@
         <v>2865</v>
       </c>
       <c r="P428" t="s">
-        <v>4583</v>
+        <v>4586</v>
       </c>
     </row>
     <row r="429" spans="7:16" x14ac:dyDescent="0.35">
@@ -22036,7 +22042,7 @@
         <v>2957</v>
       </c>
       <c r="P429" t="s">
-        <v>4584</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="430" spans="7:16" x14ac:dyDescent="0.35">
@@ -22050,7 +22056,7 @@
         <v>3801</v>
       </c>
       <c r="P430" t="s">
-        <v>4585</v>
+        <v>4588</v>
       </c>
     </row>
     <row r="431" spans="7:16" x14ac:dyDescent="0.35">
@@ -22064,7 +22070,7 @@
         <v>3802</v>
       </c>
       <c r="P431" t="s">
-        <v>4586</v>
+        <v>4589</v>
       </c>
     </row>
     <row r="432" spans="7:16" x14ac:dyDescent="0.35">
@@ -22078,7 +22084,7 @@
         <v>3803</v>
       </c>
       <c r="P432" t="s">
-        <v>4587</v>
+        <v>4590</v>
       </c>
     </row>
     <row r="433" spans="7:16" x14ac:dyDescent="0.35">
@@ -22092,7 +22098,7 @@
         <v>3804</v>
       </c>
       <c r="P433" t="s">
-        <v>4588</v>
+        <v>4591</v>
       </c>
     </row>
     <row r="434" spans="7:16" x14ac:dyDescent="0.35">
@@ -22106,7 +22112,7 @@
         <v>1039</v>
       </c>
       <c r="P434" t="s">
-        <v>4589</v>
+        <v>4592</v>
       </c>
     </row>
     <row r="435" spans="7:16" x14ac:dyDescent="0.35">
@@ -22120,7 +22126,7 @@
         <v>1183</v>
       </c>
       <c r="P435" t="s">
-        <v>4590</v>
+        <v>4593</v>
       </c>
     </row>
     <row r="436" spans="7:16" x14ac:dyDescent="0.35">
@@ -22134,7 +22140,7 @@
         <v>148</v>
       </c>
       <c r="P436" t="s">
-        <v>4591</v>
+        <v>4594</v>
       </c>
     </row>
     <row r="437" spans="7:16" x14ac:dyDescent="0.35">
@@ -22148,7 +22154,7 @@
         <v>3805</v>
       </c>
       <c r="P437" t="s">
-        <v>4592</v>
+        <v>4595</v>
       </c>
     </row>
     <row r="438" spans="7:16" x14ac:dyDescent="0.35">
@@ -22162,7 +22168,7 @@
         <v>1491</v>
       </c>
       <c r="P438" t="s">
-        <v>4593</v>
+        <v>4596</v>
       </c>
     </row>
     <row r="439" spans="7:16" x14ac:dyDescent="0.35">
@@ -22176,7 +22182,7 @@
         <v>3806</v>
       </c>
       <c r="P439" t="s">
-        <v>4594</v>
+        <v>4597</v>
       </c>
     </row>
     <row r="440" spans="7:16" x14ac:dyDescent="0.35">
@@ -22190,7 +22196,7 @@
         <v>1874</v>
       </c>
       <c r="P440" t="s">
-        <v>4595</v>
+        <v>4598</v>
       </c>
     </row>
     <row r="441" spans="7:16" x14ac:dyDescent="0.35">
@@ -22204,7 +22210,7 @@
         <v>2336</v>
       </c>
       <c r="P441" t="s">
-        <v>4596</v>
+        <v>4599</v>
       </c>
     </row>
     <row r="442" spans="7:16" x14ac:dyDescent="0.35">
@@ -22218,7 +22224,7 @@
         <v>3205</v>
       </c>
       <c r="P442" t="s">
-        <v>4597</v>
+        <v>4600</v>
       </c>
     </row>
     <row r="443" spans="7:16" x14ac:dyDescent="0.35">
@@ -22232,7 +22238,7 @@
         <v>3807</v>
       </c>
       <c r="P443" t="s">
-        <v>4598</v>
+        <v>4601</v>
       </c>
     </row>
     <row r="444" spans="7:16" x14ac:dyDescent="0.35">
@@ -22246,7 +22252,7 @@
         <v>3808</v>
       </c>
       <c r="P444" t="s">
-        <v>4599</v>
+        <v>4602</v>
       </c>
     </row>
     <row r="445" spans="7:16" x14ac:dyDescent="0.35">
@@ -22260,7 +22266,7 @@
         <v>3809</v>
       </c>
       <c r="P445" t="s">
-        <v>4600</v>
+        <v>4603</v>
       </c>
     </row>
     <row r="446" spans="7:16" x14ac:dyDescent="0.35">
@@ -22274,7 +22280,7 @@
         <v>2294</v>
       </c>
       <c r="P446" t="s">
-        <v>4601</v>
+        <v>4604</v>
       </c>
     </row>
     <row r="447" spans="7:16" x14ac:dyDescent="0.35">
@@ -22288,7 +22294,7 @@
         <v>3810</v>
       </c>
       <c r="P447" t="s">
-        <v>4602</v>
+        <v>4605</v>
       </c>
     </row>
     <row r="448" spans="7:16" x14ac:dyDescent="0.35">
@@ -22302,7 +22308,7 @@
         <v>2332</v>
       </c>
       <c r="P448" t="s">
-        <v>4603</v>
+        <v>4606</v>
       </c>
     </row>
     <row r="449" spans="7:16" x14ac:dyDescent="0.35">
@@ -22316,7 +22322,7 @@
         <v>3811</v>
       </c>
       <c r="P449" t="s">
-        <v>4604</v>
+        <v>4607</v>
       </c>
     </row>
     <row r="450" spans="7:16" x14ac:dyDescent="0.35">
@@ -22330,7 +22336,7 @@
         <v>3812</v>
       </c>
       <c r="P450" t="s">
-        <v>4605</v>
+        <v>4608</v>
       </c>
     </row>
     <row r="451" spans="7:16" x14ac:dyDescent="0.35">
@@ -22344,7 +22350,7 @@
         <v>3813</v>
       </c>
       <c r="P451" t="s">
-        <v>4606</v>
+        <v>4609</v>
       </c>
     </row>
     <row r="452" spans="7:16" x14ac:dyDescent="0.35">
@@ -22358,7 +22364,7 @@
         <v>368</v>
       </c>
       <c r="P452" t="s">
-        <v>4607</v>
+        <v>4610</v>
       </c>
     </row>
     <row r="453" spans="7:16" x14ac:dyDescent="0.35">
@@ -22372,7 +22378,7 @@
         <v>2627</v>
       </c>
       <c r="P453" t="s">
-        <v>4608</v>
+        <v>4611</v>
       </c>
     </row>
     <row r="454" spans="7:16" x14ac:dyDescent="0.35">
@@ -22386,7 +22392,7 @@
         <v>3814</v>
       </c>
       <c r="P454" t="s">
-        <v>4609</v>
+        <v>4612</v>
       </c>
     </row>
     <row r="455" spans="7:16" x14ac:dyDescent="0.35">
@@ -22400,7 +22406,7 @@
         <v>3815</v>
       </c>
       <c r="P455" t="s">
-        <v>4610</v>
+        <v>4613</v>
       </c>
     </row>
     <row r="456" spans="7:16" x14ac:dyDescent="0.35">
@@ -22413,9 +22419,6 @@
       <c r="N456" t="s">
         <v>3816</v>
       </c>
-      <c r="P456" t="s">
-        <v>4611</v>
-      </c>
     </row>
     <row r="457" spans="7:16" x14ac:dyDescent="0.35">
       <c r="G457" t="s">
@@ -22427,9 +22430,6 @@
       <c r="N457" t="s">
         <v>3817</v>
       </c>
-      <c r="P457" t="s">
-        <v>4612</v>
-      </c>
     </row>
     <row r="458" spans="7:16" x14ac:dyDescent="0.35">
       <c r="G458" t="s">
@@ -22441,9 +22441,6 @@
       <c r="N458" t="s">
         <v>3818</v>
       </c>
-      <c r="P458" t="s">
-        <v>4613</v>
-      </c>
     </row>
     <row r="459" spans="7:16" x14ac:dyDescent="0.35">
       <c r="G459" t="s">
@@ -22455,9 +22452,6 @@
       <c r="N459" t="s">
         <v>3819</v>
       </c>
-      <c r="P459" t="s">
-        <v>4614</v>
-      </c>
     </row>
     <row r="460" spans="7:16" x14ac:dyDescent="0.35">
       <c r="G460" t="s">
@@ -22468,9 +22462,6 @@
       </c>
       <c r="N460" t="s">
         <v>3820</v>
-      </c>
-      <c r="P460" t="s">
-        <v>4615</v>
       </c>
     </row>
     <row r="461" spans="7:16" x14ac:dyDescent="0.35">

</xml_diff>